<commit_message>
Did more data collection into excel. More strategy and to-do list
</commit_message>
<xml_diff>
--- a/All Other Data/s2cAllRawDataExcel.xlsx
+++ b/All Other Data/s2cAllRawDataExcel.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Name</t>
   </si>
@@ -77,9 +77,6 @@
     <t>Michelangelo</t>
   </si>
   <si>
-    <t>“I love those who can smile in trouble, who can gather strength from distress, and grow brave by reflection. ‘Tis the business of little minds to shrink, but they whose heart is firm, and whose conscience approves their conduct, will pursue their principles unto death.” </t>
-  </si>
-  <si>
     <t>A Renaissance polymath, Artist, Architect, Engineer, Inventor, Writer, Musician, Scientist, famous for his work in Anatomy. One of the greatest painters of all time. Credited with invention of helicopter, parachutes and tank. Drew The Last Supper and the Mona Lisa. His personality was considered to be "mysterious and remote".</t>
   </si>
   <si>
@@ -123,13 +120,58 @@
   </si>
   <si>
     <t>Jesus Christ</t>
+  </si>
+  <si>
+    <t>To myself I am only a child playing on the beach, while vast oceans of truth lie undiscovered before me.
+If I have seen further than others, it is by standing upon the shoulders of giants.
+I can calculate the motion of heavenly bodies, but not the madness of people.
+Truth is ever to be found in simplicity, and not in the multiplicity and confusion of things.
+To every action there is always opposed an equal reaction.
+This most beautiful system of the sun, planets and comets, could only proceed from the counsel and dominion of an intelligent and powerful Being.</t>
+  </si>
+  <si>
+    <t>Simplicity is the ultimate sophistication.
+As a well-spent day brings happy sleep, so a life well spent brings happy death.
+Learning never exhausts the mind.
+Iron rusts from disuse; stagnant water loses its purity and in cold weather becomes frozen; even so does inaction sap the vigor of the mind.
+It had long since come to my attention that people of accomplishment rarely sat back and let things happen to them. They went out and happened to things.
+“I love those who can smile in trouble, who can gather strength from distress, and grow brave by reflection. ‘Tis the business of little minds to shrink, but they whose heart is firm, and whose conscience approves their conduct, will pursue their principles unto death.” </t>
+  </si>
+  <si>
+    <t>Florence, Italy</t>
+  </si>
+  <si>
+    <t>3/6/1475</t>
+  </si>
+  <si>
+    <t>Bethlehem</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Possible Autism, Possible Asperger, Mood Disorders</t>
+  </si>
+  <si>
+    <t>Artist, Painter, Sculptor, Designer and Poet. Michelangelo was considered the greatest living artist of his time for painting, sculpture and architecture, famous for his work like the "Statue of David" and The Sistine Chapel ceiling.
+According to records, the painter was described as often paranoid, narcisstic and schizoid,  “preoccupied with his own reality" and most of the male members of his family are recorded to have exhibited similar symptoms, which might point to some genetic causes for both his brilliance and menetal disposition. Michelangelo also seems to have had difficulty forming relationships with people; he had few friends, was a loner and preferred to work independently. All of this, combined with his obvious genius in math and art, led the researchers to believe that today Michelangelo would be considered high functioning on the autism spectrum. When he was 30, he is quoted to have written, ‘Anything might happen to shatter my world.’</t>
+  </si>
+  <si>
+    <t>http://www.news-medical.net/news/2004/05/26/1931.aspx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If people knew how hard I had to work to gain my mastery, it would not seem so wonderful at all.
+I saw the angel in the marble and carved until I set him free.
+Genius is eternal patience.
+The greater danger for most of us lies not in setting our aim too high and falling short; but in setting our aim too low, and achieving our mark.
+A man paints with his brains and not with his hands.
+The true work of art is but a shadow of the divine perfection.
+Trifles make perfection, and perfection is no trifle.
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -159,10 +201,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="15"/>
       <color rgb="FF444444"/>
       <name val="Helvetica"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -203,8 +252,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -214,7 +264,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -222,14 +271,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -508,8 +561,8 @@
   <dimension ref="A1:G274"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -518,8 +571,8 @@
     <col min="2" max="2" width="23" customWidth="1"/>
     <col min="3" max="4" width="21.33203125" customWidth="1"/>
     <col min="5" max="5" width="67.5" customWidth="1"/>
-    <col min="6" max="6" width="32.5" customWidth="1"/>
-    <col min="7" max="7" width="46.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="47.33203125" customWidth="1"/>
+    <col min="7" max="7" width="46.6640625" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="31" x14ac:dyDescent="0.35">
@@ -545,7 +598,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="4" customFormat="1" ht="254" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" s="3" customFormat="1" ht="387" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -558,15 +611,17 @@
       <c r="D2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="6" t="s">
+      <c r="F2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="310" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="409.6" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -574,56 +629,68 @@
         <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="409" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="C4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+        <v>37</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="372" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -632,26 +699,26 @@
     </row>
     <row r="7" spans="1:7" ht="93" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" ht="93" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -660,11 +727,11 @@
     </row>
     <row r="9" spans="1:7" ht="93" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -3057,6 +3124,9 @@
       <c r="G274" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G4" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changing image naming scheme to Full Name. Showing correct sizes on tableview for Home Screen
</commit_message>
<xml_diff>
--- a/All Other Data/s2cAllRawDataExcel.xlsx
+++ b/All Other Data/s2cAllRawDataExcel.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Name</t>
   </si>
@@ -108,9 +108,6 @@
   </si>
   <si>
     <t>Muhammad</t>
-  </si>
-  <si>
-    <t>Joseph</t>
   </si>
   <si>
     <t>Betrayed by his own brothers</t>
@@ -166,12 +163,42 @@
 Trifles make perfection, and perfection is no trifle.
 </t>
   </si>
+  <si>
+    <t>Joseph (Bible)</t>
+  </si>
+  <si>
+    <t>Albert Einstein</t>
+  </si>
+  <si>
+    <t>3/14/1879</t>
+  </si>
+  <si>
+    <t>Ulm, Germany</t>
+  </si>
+  <si>
+    <t>http://www.famoushomeschoolers.net/bio_einstein.html#.WGLgw7YrLBI</t>
+  </si>
+  <si>
+    <t>Einstein’s parents wanted him to pursue a career in electrical engineering. Without a high school diploma, Einstein applied to the Polytechnic Institute at Zurich, Switzerland. He failed the entrance examination although he got exceptional marks in the mathematics and physics sections. Einstein described himself as “a conscientious but unassuming young man who had acquired his meagre store of pertinent knowledge of the essentials through self study. 
+He basically taught himself math and physics through books and self-study and skipped lectures and stopped going to classes that didn't interest him</t>
+  </si>
+  <si>
+    <t>Slow Learner, Late Bloomer, Possible Asperger's Syndrome, Unsociableness, Rejected from Entrance Exam</t>
+  </si>
+  <si>
+    <t>“The more I learn, the more I realize [how much] I don’t know.” “The only thing that interferes with my learning is my education.”   “I owe more to my ability to fantasize than to any knowledge I’ve ever acquired.”
+ “Example isn’t another way to teach, it is the only way to teach.”
+ “It is the supreme art of the teacher to awaken joy in creative expression and knowledge.”
+ “If you want your children to be brilliant, tell them fairy tales. If you want them to be very brilliant, tell them even more fairy tales.” “Imagination is more important than knowledge. Knowledge is limited. Imagination encircles the world.” “Why should I fill my head with things like that when I could look them up in any reference book in two minutes?”
+ “It is, in fact, nothing short of a miracle that the modern methods of instruction have not yet entirely strangled the holy curiosity of inquiry; for this delicate little plant, aside from stimulation, stands mainly in need of freedom….It is a very grave mistake to think that the enjoyment of seeing and searching can be promoted by means of coercion and a sense of duty.”
+“The problem involved is too vast for our limited minds. We are in the position of a little child entering a huge library filled with books in many languages. The child knows someone must have written those books. It does not know how. It does not understand the languages in which they are written. The child dimly suspects a mysterious order in the arrangement of the books but doesn't know what it is. That, it seems to me, is the attitude of even the most intelligent human being toward God. We see the universe marvelously arranged and obeying certain laws but only dimly understand these laws.”</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -212,6 +239,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Times"/>
     </font>
   </fonts>
   <fills count="3">
@@ -256,7 +288,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -279,6 +311,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -560,16 +595,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G274"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="48.1640625" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="4" width="21.33203125" customWidth="1"/>
+    <col min="3" max="3" width="34" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" customWidth="1"/>
     <col min="5" max="5" width="67.5" customWidth="1"/>
     <col min="6" max="6" width="47.33203125" customWidth="1"/>
     <col min="7" max="7" width="46.6640625" style="6" bestFit="1" customWidth="1"/>
@@ -598,7 +634,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="3" customFormat="1" ht="387" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" s="3" customFormat="1" ht="291" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -615,7 +651,7 @@
         <v>10</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>9</v>
@@ -638,7 +674,7 @@
         <v>17</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G3" s="2"/>
     </row>
@@ -647,27 +683,27 @@
         <v>16</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="8" t="s">
         <v>38</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="372" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>19</v>
@@ -676,7 +712,7 @@
         <v>20</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>21</v>
@@ -718,34 +754,48 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" ht="93" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="62" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+    <row r="10" spans="1:7" ht="409" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
@@ -3128,5 +3178,6 @@
     <hyperlink ref="G4" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update: Clean up comments, add pics for Picasso, Van Gogh, add more excel entries
</commit_message>
<xml_diff>
--- a/All Other Data/s2cAllRawDataExcel.xlsx
+++ b/All Other Data/s2cAllRawDataExcel.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="71">
   <si>
     <t>Name</t>
   </si>
@@ -71,9 +71,6 @@
     <t>England</t>
   </si>
   <si>
-    <t>Italy</t>
-  </si>
-  <si>
     <t>Michelangelo</t>
   </si>
   <si>
@@ -83,12 +80,6 @@
     <t>Lack of Formal Education</t>
   </si>
   <si>
-    <t>???</t>
-  </si>
-  <si>
-    <t>Betrayal, Suicidal Thoughts</t>
-  </si>
-  <si>
     <t xml:space="preserve">Apparently in the Temptation of Christ, Devil whispered in his ears to jump off. Not sure if he was hallucinating or severely depressed but even Christ had suicidal thoughts and nasty Devil in his ear. He was also betrayed by one of his disciples and unjustly killed by others who framed him as a false King and was nailed to the cross. But after his death, we still know that Jesus existed 2000 years ago and we sing of his wisdom 2000 years later. Who won? </t>
   </si>
   <si>
@@ -108,9 +99,6 @@
   </si>
   <si>
     <t>Muhammad</t>
-  </si>
-  <si>
-    <t>Betrayed by his own brothers</t>
   </si>
   <si>
     <t>Losing parents at early age</t>
@@ -139,12 +127,6 @@
   </si>
   <si>
     <t>3/6/1475</t>
-  </si>
-  <si>
-    <t>Bethlehem</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Possible Autism, Possible Asperger, Mood Disorders</t>
   </si>
   <si>
     <t>Artist, Painter, Sculptor, Designer and Poet. Michelangelo was considered the greatest living artist of his time for painting, sculpture and architecture, famous for his work like the "Statue of David" and The Sistine Chapel ceiling.
@@ -164,9 +146,6 @@
 </t>
   </si>
   <si>
-    <t>Joseph (Bible)</t>
-  </si>
-  <si>
     <t>Albert Einstein</t>
   </si>
   <si>
@@ -192,6 +171,97 @@
  “If you want your children to be brilliant, tell them fairy tales. If you want them to be very brilliant, tell them even more fairy tales.” “Imagination is more important than knowledge. Knowledge is limited. Imagination encircles the world.” “Why should I fill my head with things like that when I could look them up in any reference book in two minutes?”
  “It is, in fact, nothing short of a miracle that the modern methods of instruction have not yet entirely strangled the holy curiosity of inquiry; for this delicate little plant, aside from stimulation, stands mainly in need of freedom….It is a very grave mistake to think that the enjoyment of seeing and searching can be promoted by means of coercion and a sense of duty.”
 “The problem involved is too vast for our limited minds. We are in the position of a little child entering a huge library filled with books in many languages. The child knows someone must have written those books. It does not know how. It does not understand the languages in which they are written. The child dimly suspects a mysterious order in the arrangement of the books but doesn't know what it is. That, it seems to me, is the attitude of even the most intelligent human being toward God. We see the universe marvelously arranged and obeying certain laws but only dimly understand these laws.”</t>
+  </si>
+  <si>
+    <t>Pablo Picasso</t>
+  </si>
+  <si>
+    <t>"The meaning of life is to find your gift. The purpose of life is to give it away"
+"God is really another artist. He invented the giraffe, the elephant, and the cat. He has no real style. He just goes on trying other things"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Possible OCD, Possible Autism, Possible Asperger, Mood Disorders</t>
+  </si>
+  <si>
+    <t>Vincent van Gogh</t>
+  </si>
+  <si>
+    <t>Depression, Bipolar, Suicidal Thoughts</t>
+  </si>
+  <si>
+    <t>Nikola Tesla</t>
+  </si>
+  <si>
+    <t>OCD</t>
+  </si>
+  <si>
+    <t>7/10/1856</t>
+  </si>
+  <si>
+    <t>David Beckham</t>
+  </si>
+  <si>
+    <t>Justin Timberlake</t>
+  </si>
+  <si>
+    <t>OCD, ADHD</t>
+  </si>
+  <si>
+    <t>Martin Scorsese</t>
+  </si>
+  <si>
+    <t>Malaga, Spain</t>
+  </si>
+  <si>
+    <t>10/25/1881</t>
+  </si>
+  <si>
+    <t>3/30/1853</t>
+  </si>
+  <si>
+    <t>Zundert, Netherlands</t>
+  </si>
+  <si>
+    <t>4-6 BCE</t>
+  </si>
+  <si>
+    <t>2/12/1809</t>
+  </si>
+  <si>
+    <t>Hodgenville, KY</t>
+  </si>
+  <si>
+    <t>Atlanta, GA</t>
+  </si>
+  <si>
+    <t>Mecca, Saudi Arabia</t>
+  </si>
+  <si>
+    <t>Bethlehem, Palestine</t>
+  </si>
+  <si>
+    <t>Anciano, Italy</t>
+  </si>
+  <si>
+    <t>Joseph</t>
+  </si>
+  <si>
+    <t>http://www.myjewishlearning.com/article/the-story-of-joseph/</t>
+  </si>
+  <si>
+    <t>Betrayal, Falsely Accused, Slandered, Persecuted, Humiliated, Suicidal Thoughts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Betrayal, Falsely Accused, Slavery </t>
+  </si>
+  <si>
+    <t>Before the time of Moses</t>
+  </si>
+  <si>
+    <t>The story of Joseph is found in the Book of Genesis in the Torah &amp; Bible. His life was a series of highs and lows. He was the most favored son and most loved by his father, Jacob, among his 10 brothers. Not only that, he was talented at interpreting dreams and prophesized that one day he will rule over his family. His life took a major downturn when his jealous brothers captured him and sold him into slavery at Egypt, faking his death. As a slave, his intelligence and talent quickly promoted him as head of all the slaves but at one point, his owner's wife tried to seduce him and then accused him of rape which got him thrown out. After years in slavery and prison cells, he eventually gained audience with the Pharaoh of Egypt by interpreting his dreams and predicting that a great famine was to come. The Pharaoh was impressed with him and made Joseph into a Vizier, second-in-command of all of Egypt.  Joseph's brothers, 20 years after selling Joseph to slavery, went down to Egypt after suffering from famine, and met Joseph who was now very powerful. Joseph forgave his brothers and brougth the entire family down to Egypt. Joseph lives until 110 years old, and his will was for the Jews to take his remains with them when they finally leave Egypt. Moses fulfills his wills by carrying Joseph's bones on the way to Israel.</t>
+  </si>
+  <si>
+    <t>Canaan</t>
   </si>
 </sst>
 </file>
@@ -288,7 +358,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -315,6 +385,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -595,15 +672,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G274"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="48.1640625" customWidth="1"/>
-    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" style="12" customWidth="1"/>
     <col min="3" max="3" width="34" customWidth="1"/>
     <col min="4" max="4" width="21.33203125" customWidth="1"/>
     <col min="5" max="5" width="67.5" customWidth="1"/>
@@ -615,7 +692,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -638,7 +715,7 @@
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="10" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -651,7 +728,7 @@
         <v>10</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>9</v>
@@ -661,191 +738,247 @@
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="10" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" ht="409" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>34</v>
+        <v>15</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>30</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="G4" s="8" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="372" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>19</v>
+        <v>26</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>57</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="62" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="2"/>
+        <v>19</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>58</v>
+      </c>
       <c r="C6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="2"/>
+        <v>20</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="93" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="62" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="B7" s="10">
+        <v>10608</v>
+      </c>
       <c r="C7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="2"/>
+        <v>22</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="E7" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" ht="93" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="B8" s="10"/>
       <c r="C8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" ht="62" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="409" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="C9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+        <v>67</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
+      <c r="G9" s="8" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="409" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="248" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B11" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E10" s="9" t="s">
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" ht="93" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
+      <c r="A13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
+      <c r="A14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="10"/>
+      <c r="C14" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
+      <c r="A15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="10"/>
+      <c r="C15" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+      <c r="A16" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="10">
+        <v>15662</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -853,7 +986,7 @@
     </row>
     <row r="17" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
+      <c r="B17" s="10"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -862,7 +995,7 @@
     </row>
     <row r="18" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
+      <c r="B18" s="10"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -871,7 +1004,7 @@
     </row>
     <row r="19" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
+      <c r="B19" s="10"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -880,7 +1013,7 @@
     </row>
     <row r="20" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
+      <c r="B20" s="10"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -889,7 +1022,7 @@
     </row>
     <row r="21" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
+      <c r="B21" s="10"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -898,7 +1031,7 @@
     </row>
     <row r="22" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
+      <c r="B22" s="10"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -907,7 +1040,7 @@
     </row>
     <row r="23" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
+      <c r="B23" s="10"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -916,7 +1049,7 @@
     </row>
     <row r="24" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
+      <c r="B24" s="10"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -925,7 +1058,7 @@
     </row>
     <row r="25" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
+      <c r="B25" s="10"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -934,7 +1067,7 @@
     </row>
     <row r="26" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
+      <c r="B26" s="10"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -943,7 +1076,7 @@
     </row>
     <row r="27" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
+      <c r="B27" s="10"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -952,7 +1085,7 @@
     </row>
     <row r="28" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
+      <c r="B28" s="10"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -961,7 +1094,7 @@
     </row>
     <row r="29" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
+      <c r="B29" s="10"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -970,7 +1103,7 @@
     </row>
     <row r="30" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
+      <c r="B30" s="10"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -979,7 +1112,7 @@
     </row>
     <row r="31" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
+      <c r="B31" s="10"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -988,7 +1121,7 @@
     </row>
     <row r="32" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
+      <c r="B32" s="10"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -997,7 +1130,7 @@
     </row>
     <row r="33" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
+      <c r="B33" s="10"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -1006,7 +1139,7 @@
     </row>
     <row r="34" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
+      <c r="B34" s="10"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -1015,7 +1148,7 @@
     </row>
     <row r="35" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
+      <c r="B35" s="10"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -1024,7 +1157,7 @@
     </row>
     <row r="36" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
+      <c r="B36" s="10"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -1033,7 +1166,7 @@
     </row>
     <row r="37" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
+      <c r="B37" s="10"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -1042,7 +1175,7 @@
     </row>
     <row r="38" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
+      <c r="B38" s="10"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
@@ -1051,7 +1184,7 @@
     </row>
     <row r="39" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
+      <c r="B39" s="10"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
@@ -1060,7 +1193,7 @@
     </row>
     <row r="40" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
+      <c r="B40" s="10"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -1069,7 +1202,7 @@
     </row>
     <row r="41" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
+      <c r="B41" s="10"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -1078,7 +1211,7 @@
     </row>
     <row r="42" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
+      <c r="B42" s="10"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -1087,7 +1220,7 @@
     </row>
     <row r="43" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
+      <c r="B43" s="10"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
@@ -1096,7 +1229,7 @@
     </row>
     <row r="44" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A44" s="2"/>
-      <c r="B44" s="2"/>
+      <c r="B44" s="10"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
@@ -1105,7 +1238,7 @@
     </row>
     <row r="45" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
+      <c r="B45" s="10"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -1114,7 +1247,7 @@
     </row>
     <row r="46" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A46" s="2"/>
-      <c r="B46" s="2"/>
+      <c r="B46" s="10"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
@@ -1123,7 +1256,7 @@
     </row>
     <row r="47" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A47" s="2"/>
-      <c r="B47" s="2"/>
+      <c r="B47" s="10"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
@@ -1132,7 +1265,7 @@
     </row>
     <row r="48" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A48" s="2"/>
-      <c r="B48" s="2"/>
+      <c r="B48" s="10"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
@@ -1141,7 +1274,7 @@
     </row>
     <row r="49" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A49" s="2"/>
-      <c r="B49" s="2"/>
+      <c r="B49" s="10"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
@@ -1150,7 +1283,7 @@
     </row>
     <row r="50" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A50" s="2"/>
-      <c r="B50" s="2"/>
+      <c r="B50" s="10"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
@@ -1159,7 +1292,7 @@
     </row>
     <row r="51" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A51" s="2"/>
-      <c r="B51" s="2"/>
+      <c r="B51" s="10"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
@@ -1168,7 +1301,7 @@
     </row>
     <row r="52" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A52" s="2"/>
-      <c r="B52" s="2"/>
+      <c r="B52" s="10"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
@@ -1177,7 +1310,7 @@
     </row>
     <row r="53" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A53" s="2"/>
-      <c r="B53" s="2"/>
+      <c r="B53" s="10"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
@@ -1186,7 +1319,7 @@
     </row>
     <row r="54" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A54" s="2"/>
-      <c r="B54" s="2"/>
+      <c r="B54" s="10"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
@@ -1195,7 +1328,7 @@
     </row>
     <row r="55" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A55" s="2"/>
-      <c r="B55" s="2"/>
+      <c r="B55" s="10"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
@@ -1204,7 +1337,7 @@
     </row>
     <row r="56" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A56" s="2"/>
-      <c r="B56" s="2"/>
+      <c r="B56" s="10"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
@@ -1213,7 +1346,7 @@
     </row>
     <row r="57" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A57" s="2"/>
-      <c r="B57" s="2"/>
+      <c r="B57" s="10"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
@@ -1222,7 +1355,7 @@
     </row>
     <row r="58" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A58" s="2"/>
-      <c r="B58" s="2"/>
+      <c r="B58" s="10"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
@@ -1231,7 +1364,7 @@
     </row>
     <row r="59" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A59" s="2"/>
-      <c r="B59" s="2"/>
+      <c r="B59" s="10"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
@@ -1240,7 +1373,7 @@
     </row>
     <row r="60" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A60" s="2"/>
-      <c r="B60" s="2"/>
+      <c r="B60" s="10"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
@@ -1249,7 +1382,7 @@
     </row>
     <row r="61" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A61" s="2"/>
-      <c r="B61" s="2"/>
+      <c r="B61" s="10"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
@@ -1258,7 +1391,7 @@
     </row>
     <row r="62" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A62" s="2"/>
-      <c r="B62" s="2"/>
+      <c r="B62" s="10"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
@@ -1267,7 +1400,7 @@
     </row>
     <row r="63" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A63" s="2"/>
-      <c r="B63" s="2"/>
+      <c r="B63" s="10"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
@@ -1276,7 +1409,7 @@
     </row>
     <row r="64" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A64" s="2"/>
-      <c r="B64" s="2"/>
+      <c r="B64" s="10"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
@@ -1285,7 +1418,7 @@
     </row>
     <row r="65" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A65" s="2"/>
-      <c r="B65" s="2"/>
+      <c r="B65" s="10"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
@@ -1294,7 +1427,7 @@
     </row>
     <row r="66" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A66" s="2"/>
-      <c r="B66" s="2"/>
+      <c r="B66" s="10"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
@@ -1303,7 +1436,7 @@
     </row>
     <row r="67" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A67" s="2"/>
-      <c r="B67" s="2"/>
+      <c r="B67" s="10"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
@@ -1312,7 +1445,7 @@
     </row>
     <row r="68" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A68" s="2"/>
-      <c r="B68" s="2"/>
+      <c r="B68" s="10"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
@@ -1321,7 +1454,7 @@
     </row>
     <row r="69" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A69" s="2"/>
-      <c r="B69" s="2"/>
+      <c r="B69" s="10"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
@@ -1330,7 +1463,7 @@
     </row>
     <row r="70" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A70" s="2"/>
-      <c r="B70" s="2"/>
+      <c r="B70" s="10"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
@@ -1339,7 +1472,7 @@
     </row>
     <row r="71" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A71" s="2"/>
-      <c r="B71" s="2"/>
+      <c r="B71" s="10"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
@@ -1348,7 +1481,7 @@
     </row>
     <row r="72" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A72" s="2"/>
-      <c r="B72" s="2"/>
+      <c r="B72" s="10"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
@@ -1357,7 +1490,7 @@
     </row>
     <row r="73" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A73" s="2"/>
-      <c r="B73" s="2"/>
+      <c r="B73" s="10"/>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
       <c r="E73" s="2"/>
@@ -1366,7 +1499,7 @@
     </row>
     <row r="74" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A74" s="2"/>
-      <c r="B74" s="2"/>
+      <c r="B74" s="10"/>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
       <c r="E74" s="2"/>
@@ -1375,7 +1508,7 @@
     </row>
     <row r="75" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A75" s="2"/>
-      <c r="B75" s="2"/>
+      <c r="B75" s="10"/>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
       <c r="E75" s="2"/>
@@ -1384,7 +1517,7 @@
     </row>
     <row r="76" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A76" s="2"/>
-      <c r="B76" s="2"/>
+      <c r="B76" s="10"/>
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
       <c r="E76" s="2"/>
@@ -1393,7 +1526,7 @@
     </row>
     <row r="77" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A77" s="2"/>
-      <c r="B77" s="2"/>
+      <c r="B77" s="10"/>
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
       <c r="E77" s="2"/>
@@ -1402,7 +1535,7 @@
     </row>
     <row r="78" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A78" s="2"/>
-      <c r="B78" s="2"/>
+      <c r="B78" s="10"/>
       <c r="C78" s="2"/>
       <c r="D78" s="2"/>
       <c r="E78" s="2"/>
@@ -1411,7 +1544,7 @@
     </row>
     <row r="79" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A79" s="2"/>
-      <c r="B79" s="2"/>
+      <c r="B79" s="10"/>
       <c r="C79" s="2"/>
       <c r="D79" s="2"/>
       <c r="E79" s="2"/>
@@ -1420,7 +1553,7 @@
     </row>
     <row r="80" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A80" s="2"/>
-      <c r="B80" s="2"/>
+      <c r="B80" s="10"/>
       <c r="C80" s="2"/>
       <c r="D80" s="2"/>
       <c r="E80" s="2"/>
@@ -1429,7 +1562,7 @@
     </row>
     <row r="81" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A81" s="2"/>
-      <c r="B81" s="2"/>
+      <c r="B81" s="10"/>
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
       <c r="E81" s="2"/>
@@ -1438,7 +1571,7 @@
     </row>
     <row r="82" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A82" s="2"/>
-      <c r="B82" s="2"/>
+      <c r="B82" s="10"/>
       <c r="C82" s="2"/>
       <c r="D82" s="2"/>
       <c r="E82" s="2"/>
@@ -1447,7 +1580,7 @@
     </row>
     <row r="83" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A83" s="2"/>
-      <c r="B83" s="2"/>
+      <c r="B83" s="10"/>
       <c r="C83" s="2"/>
       <c r="D83" s="2"/>
       <c r="E83" s="2"/>
@@ -1456,7 +1589,7 @@
     </row>
     <row r="84" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A84" s="2"/>
-      <c r="B84" s="2"/>
+      <c r="B84" s="10"/>
       <c r="C84" s="2"/>
       <c r="D84" s="2"/>
       <c r="E84" s="2"/>
@@ -1465,7 +1598,7 @@
     </row>
     <row r="85" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A85" s="2"/>
-      <c r="B85" s="2"/>
+      <c r="B85" s="10"/>
       <c r="C85" s="2"/>
       <c r="D85" s="2"/>
       <c r="E85" s="2"/>
@@ -1474,7 +1607,7 @@
     </row>
     <row r="86" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A86" s="2"/>
-      <c r="B86" s="2"/>
+      <c r="B86" s="10"/>
       <c r="C86" s="2"/>
       <c r="D86" s="2"/>
       <c r="E86" s="2"/>
@@ -1483,7 +1616,7 @@
     </row>
     <row r="87" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A87" s="2"/>
-      <c r="B87" s="2"/>
+      <c r="B87" s="10"/>
       <c r="C87" s="2"/>
       <c r="D87" s="2"/>
       <c r="E87" s="2"/>
@@ -1492,7 +1625,7 @@
     </row>
     <row r="88" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A88" s="2"/>
-      <c r="B88" s="2"/>
+      <c r="B88" s="10"/>
       <c r="C88" s="2"/>
       <c r="D88" s="2"/>
       <c r="E88" s="2"/>
@@ -1501,7 +1634,7 @@
     </row>
     <row r="89" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A89" s="2"/>
-      <c r="B89" s="2"/>
+      <c r="B89" s="10"/>
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
       <c r="E89" s="2"/>
@@ -1510,7 +1643,7 @@
     </row>
     <row r="90" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A90" s="2"/>
-      <c r="B90" s="2"/>
+      <c r="B90" s="10"/>
       <c r="C90" s="2"/>
       <c r="D90" s="2"/>
       <c r="E90" s="2"/>
@@ -1519,7 +1652,7 @@
     </row>
     <row r="91" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A91" s="2"/>
-      <c r="B91" s="2"/>
+      <c r="B91" s="10"/>
       <c r="C91" s="2"/>
       <c r="D91" s="2"/>
       <c r="E91" s="2"/>
@@ -1528,7 +1661,7 @@
     </row>
     <row r="92" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A92" s="2"/>
-      <c r="B92" s="2"/>
+      <c r="B92" s="10"/>
       <c r="C92" s="2"/>
       <c r="D92" s="2"/>
       <c r="E92" s="2"/>
@@ -1537,7 +1670,7 @@
     </row>
     <row r="93" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A93" s="2"/>
-      <c r="B93" s="2"/>
+      <c r="B93" s="10"/>
       <c r="C93" s="2"/>
       <c r="D93" s="2"/>
       <c r="E93" s="2"/>
@@ -1546,7 +1679,7 @@
     </row>
     <row r="94" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A94" s="2"/>
-      <c r="B94" s="2"/>
+      <c r="B94" s="10"/>
       <c r="C94" s="2"/>
       <c r="D94" s="2"/>
       <c r="E94" s="2"/>
@@ -1555,7 +1688,7 @@
     </row>
     <row r="95" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A95" s="2"/>
-      <c r="B95" s="2"/>
+      <c r="B95" s="10"/>
       <c r="C95" s="2"/>
       <c r="D95" s="2"/>
       <c r="E95" s="2"/>
@@ -1564,7 +1697,7 @@
     </row>
     <row r="96" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A96" s="2"/>
-      <c r="B96" s="2"/>
+      <c r="B96" s="10"/>
       <c r="C96" s="2"/>
       <c r="D96" s="2"/>
       <c r="E96" s="2"/>
@@ -1573,7 +1706,7 @@
     </row>
     <row r="97" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A97" s="2"/>
-      <c r="B97" s="2"/>
+      <c r="B97" s="10"/>
       <c r="C97" s="2"/>
       <c r="D97" s="2"/>
       <c r="E97" s="2"/>
@@ -1582,7 +1715,7 @@
     </row>
     <row r="98" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A98" s="2"/>
-      <c r="B98" s="2"/>
+      <c r="B98" s="10"/>
       <c r="C98" s="2"/>
       <c r="D98" s="2"/>
       <c r="E98" s="2"/>
@@ -1591,7 +1724,7 @@
     </row>
     <row r="99" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A99" s="2"/>
-      <c r="B99" s="2"/>
+      <c r="B99" s="10"/>
       <c r="C99" s="2"/>
       <c r="D99" s="2"/>
       <c r="E99" s="2"/>
@@ -1600,7 +1733,7 @@
     </row>
     <row r="100" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A100" s="2"/>
-      <c r="B100" s="2"/>
+      <c r="B100" s="10"/>
       <c r="C100" s="2"/>
       <c r="D100" s="2"/>
       <c r="E100" s="2"/>
@@ -1609,7 +1742,7 @@
     </row>
     <row r="101" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A101" s="2"/>
-      <c r="B101" s="2"/>
+      <c r="B101" s="10"/>
       <c r="C101" s="2"/>
       <c r="D101" s="2"/>
       <c r="E101" s="2"/>
@@ -1618,7 +1751,7 @@
     </row>
     <row r="102" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A102" s="2"/>
-      <c r="B102" s="2"/>
+      <c r="B102" s="10"/>
       <c r="C102" s="2"/>
       <c r="D102" s="2"/>
       <c r="E102" s="2"/>
@@ -1627,7 +1760,7 @@
     </row>
     <row r="103" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A103" s="2"/>
-      <c r="B103" s="2"/>
+      <c r="B103" s="10"/>
       <c r="C103" s="2"/>
       <c r="D103" s="2"/>
       <c r="E103" s="2"/>
@@ -1636,7 +1769,7 @@
     </row>
     <row r="104" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A104" s="2"/>
-      <c r="B104" s="2"/>
+      <c r="B104" s="10"/>
       <c r="C104" s="2"/>
       <c r="D104" s="2"/>
       <c r="E104" s="2"/>
@@ -1645,7 +1778,7 @@
     </row>
     <row r="105" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A105" s="2"/>
-      <c r="B105" s="2"/>
+      <c r="B105" s="10"/>
       <c r="C105" s="2"/>
       <c r="D105" s="2"/>
       <c r="E105" s="2"/>
@@ -1654,7 +1787,7 @@
     </row>
     <row r="106" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A106" s="2"/>
-      <c r="B106" s="2"/>
+      <c r="B106" s="10"/>
       <c r="C106" s="2"/>
       <c r="D106" s="2"/>
       <c r="E106" s="2"/>
@@ -1663,7 +1796,7 @@
     </row>
     <row r="107" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A107" s="2"/>
-      <c r="B107" s="2"/>
+      <c r="B107" s="10"/>
       <c r="C107" s="2"/>
       <c r="D107" s="2"/>
       <c r="E107" s="2"/>
@@ -1672,7 +1805,7 @@
     </row>
     <row r="108" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A108" s="2"/>
-      <c r="B108" s="2"/>
+      <c r="B108" s="10"/>
       <c r="C108" s="2"/>
       <c r="D108" s="2"/>
       <c r="E108" s="2"/>
@@ -1681,7 +1814,7 @@
     </row>
     <row r="109" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A109" s="2"/>
-      <c r="B109" s="2"/>
+      <c r="B109" s="10"/>
       <c r="C109" s="2"/>
       <c r="D109" s="2"/>
       <c r="E109" s="2"/>
@@ -1690,7 +1823,7 @@
     </row>
     <row r="110" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A110" s="2"/>
-      <c r="B110" s="2"/>
+      <c r="B110" s="10"/>
       <c r="C110" s="2"/>
       <c r="D110" s="2"/>
       <c r="E110" s="2"/>
@@ -1699,7 +1832,7 @@
     </row>
     <row r="111" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A111" s="2"/>
-      <c r="B111" s="2"/>
+      <c r="B111" s="10"/>
       <c r="C111" s="2"/>
       <c r="D111" s="2"/>
       <c r="E111" s="2"/>
@@ -1708,7 +1841,7 @@
     </row>
     <row r="112" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A112" s="2"/>
-      <c r="B112" s="2"/>
+      <c r="B112" s="10"/>
       <c r="C112" s="2"/>
       <c r="D112" s="2"/>
       <c r="E112" s="2"/>
@@ -1717,7 +1850,7 @@
     </row>
     <row r="113" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A113" s="2"/>
-      <c r="B113" s="2"/>
+      <c r="B113" s="10"/>
       <c r="C113" s="2"/>
       <c r="D113" s="2"/>
       <c r="E113" s="2"/>
@@ -1726,7 +1859,7 @@
     </row>
     <row r="114" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A114" s="2"/>
-      <c r="B114" s="2"/>
+      <c r="B114" s="10"/>
       <c r="C114" s="2"/>
       <c r="D114" s="2"/>
       <c r="E114" s="2"/>
@@ -1735,7 +1868,7 @@
     </row>
     <row r="115" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A115" s="2"/>
-      <c r="B115" s="2"/>
+      <c r="B115" s="10"/>
       <c r="C115" s="2"/>
       <c r="D115" s="2"/>
       <c r="E115" s="2"/>
@@ -1744,7 +1877,7 @@
     </row>
     <row r="116" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A116" s="2"/>
-      <c r="B116" s="2"/>
+      <c r="B116" s="10"/>
       <c r="C116" s="2"/>
       <c r="D116" s="2"/>
       <c r="E116" s="2"/>
@@ -1753,7 +1886,7 @@
     </row>
     <row r="117" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A117" s="2"/>
-      <c r="B117" s="2"/>
+      <c r="B117" s="10"/>
       <c r="C117" s="2"/>
       <c r="D117" s="2"/>
       <c r="E117" s="2"/>
@@ -1762,7 +1895,7 @@
     </row>
     <row r="118" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A118" s="2"/>
-      <c r="B118" s="2"/>
+      <c r="B118" s="10"/>
       <c r="C118" s="2"/>
       <c r="D118" s="2"/>
       <c r="E118" s="2"/>
@@ -1771,7 +1904,7 @@
     </row>
     <row r="119" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A119" s="2"/>
-      <c r="B119" s="2"/>
+      <c r="B119" s="10"/>
       <c r="C119" s="2"/>
       <c r="D119" s="2"/>
       <c r="E119" s="2"/>
@@ -1780,7 +1913,7 @@
     </row>
     <row r="120" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A120" s="2"/>
-      <c r="B120" s="2"/>
+      <c r="B120" s="10"/>
       <c r="C120" s="2"/>
       <c r="D120" s="2"/>
       <c r="E120" s="2"/>
@@ -1789,7 +1922,7 @@
     </row>
     <row r="121" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A121" s="2"/>
-      <c r="B121" s="2"/>
+      <c r="B121" s="10"/>
       <c r="C121" s="2"/>
       <c r="D121" s="2"/>
       <c r="E121" s="2"/>
@@ -1798,7 +1931,7 @@
     </row>
     <row r="122" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A122" s="2"/>
-      <c r="B122" s="2"/>
+      <c r="B122" s="10"/>
       <c r="C122" s="2"/>
       <c r="D122" s="2"/>
       <c r="E122" s="2"/>
@@ -1807,7 +1940,7 @@
     </row>
     <row r="123" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A123" s="2"/>
-      <c r="B123" s="2"/>
+      <c r="B123" s="10"/>
       <c r="C123" s="2"/>
       <c r="D123" s="2"/>
       <c r="E123" s="2"/>
@@ -1816,7 +1949,7 @@
     </row>
     <row r="124" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A124" s="2"/>
-      <c r="B124" s="2"/>
+      <c r="B124" s="10"/>
       <c r="C124" s="2"/>
       <c r="D124" s="2"/>
       <c r="E124" s="2"/>
@@ -1825,7 +1958,7 @@
     </row>
     <row r="125" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A125" s="2"/>
-      <c r="B125" s="2"/>
+      <c r="B125" s="10"/>
       <c r="C125" s="2"/>
       <c r="D125" s="2"/>
       <c r="E125" s="2"/>
@@ -1834,7 +1967,7 @@
     </row>
     <row r="126" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A126" s="2"/>
-      <c r="B126" s="2"/>
+      <c r="B126" s="10"/>
       <c r="C126" s="2"/>
       <c r="D126" s="2"/>
       <c r="E126" s="2"/>
@@ -1843,7 +1976,7 @@
     </row>
     <row r="127" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A127" s="2"/>
-      <c r="B127" s="2"/>
+      <c r="B127" s="10"/>
       <c r="C127" s="2"/>
       <c r="D127" s="2"/>
       <c r="E127" s="2"/>
@@ -1852,7 +1985,7 @@
     </row>
     <row r="128" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A128" s="2"/>
-      <c r="B128" s="2"/>
+      <c r="B128" s="10"/>
       <c r="C128" s="2"/>
       <c r="D128" s="2"/>
       <c r="E128" s="2"/>
@@ -1861,7 +1994,7 @@
     </row>
     <row r="129" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A129" s="2"/>
-      <c r="B129" s="2"/>
+      <c r="B129" s="10"/>
       <c r="C129" s="2"/>
       <c r="D129" s="2"/>
       <c r="E129" s="2"/>
@@ -1870,7 +2003,7 @@
     </row>
     <row r="130" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A130" s="2"/>
-      <c r="B130" s="2"/>
+      <c r="B130" s="10"/>
       <c r="C130" s="2"/>
       <c r="D130" s="2"/>
       <c r="E130" s="2"/>
@@ -1879,7 +2012,7 @@
     </row>
     <row r="131" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A131" s="2"/>
-      <c r="B131" s="2"/>
+      <c r="B131" s="10"/>
       <c r="C131" s="2"/>
       <c r="D131" s="2"/>
       <c r="E131" s="2"/>
@@ -1888,7 +2021,7 @@
     </row>
     <row r="132" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A132" s="2"/>
-      <c r="B132" s="2"/>
+      <c r="B132" s="10"/>
       <c r="C132" s="2"/>
       <c r="D132" s="2"/>
       <c r="E132" s="2"/>
@@ -1897,7 +2030,7 @@
     </row>
     <row r="133" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A133" s="2"/>
-      <c r="B133" s="2"/>
+      <c r="B133" s="10"/>
       <c r="C133" s="2"/>
       <c r="D133" s="2"/>
       <c r="E133" s="2"/>
@@ -1906,7 +2039,7 @@
     </row>
     <row r="134" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A134" s="2"/>
-      <c r="B134" s="2"/>
+      <c r="B134" s="10"/>
       <c r="C134" s="2"/>
       <c r="D134" s="2"/>
       <c r="E134" s="2"/>
@@ -1915,7 +2048,7 @@
     </row>
     <row r="135" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A135" s="2"/>
-      <c r="B135" s="2"/>
+      <c r="B135" s="10"/>
       <c r="C135" s="2"/>
       <c r="D135" s="2"/>
       <c r="E135" s="2"/>
@@ -1924,7 +2057,7 @@
     </row>
     <row r="136" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A136" s="2"/>
-      <c r="B136" s="2"/>
+      <c r="B136" s="10"/>
       <c r="C136" s="2"/>
       <c r="D136" s="2"/>
       <c r="E136" s="2"/>
@@ -1933,7 +2066,7 @@
     </row>
     <row r="137" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A137" s="2"/>
-      <c r="B137" s="2"/>
+      <c r="B137" s="10"/>
       <c r="C137" s="2"/>
       <c r="D137" s="2"/>
       <c r="E137" s="2"/>
@@ -1942,7 +2075,7 @@
     </row>
     <row r="138" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A138" s="2"/>
-      <c r="B138" s="2"/>
+      <c r="B138" s="10"/>
       <c r="C138" s="2"/>
       <c r="D138" s="2"/>
       <c r="E138" s="2"/>
@@ -1951,7 +2084,7 @@
     </row>
     <row r="139" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A139" s="2"/>
-      <c r="B139" s="2"/>
+      <c r="B139" s="10"/>
       <c r="C139" s="2"/>
       <c r="D139" s="2"/>
       <c r="E139" s="2"/>
@@ -1960,7 +2093,7 @@
     </row>
     <row r="140" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A140" s="2"/>
-      <c r="B140" s="2"/>
+      <c r="B140" s="10"/>
       <c r="C140" s="2"/>
       <c r="D140" s="2"/>
       <c r="E140" s="2"/>
@@ -1969,7 +2102,7 @@
     </row>
     <row r="141" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A141" s="2"/>
-      <c r="B141" s="2"/>
+      <c r="B141" s="10"/>
       <c r="C141" s="2"/>
       <c r="D141" s="2"/>
       <c r="E141" s="2"/>
@@ -1978,7 +2111,7 @@
     </row>
     <row r="142" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A142" s="2"/>
-      <c r="B142" s="2"/>
+      <c r="B142" s="10"/>
       <c r="C142" s="2"/>
       <c r="D142" s="2"/>
       <c r="E142" s="2"/>
@@ -1987,7 +2120,7 @@
     </row>
     <row r="143" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A143" s="2"/>
-      <c r="B143" s="2"/>
+      <c r="B143" s="10"/>
       <c r="C143" s="2"/>
       <c r="D143" s="2"/>
       <c r="E143" s="2"/>
@@ -1996,7 +2129,7 @@
     </row>
     <row r="144" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A144" s="2"/>
-      <c r="B144" s="2"/>
+      <c r="B144" s="10"/>
       <c r="C144" s="2"/>
       <c r="D144" s="2"/>
       <c r="E144" s="2"/>
@@ -2005,7 +2138,7 @@
     </row>
     <row r="145" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A145" s="2"/>
-      <c r="B145" s="2"/>
+      <c r="B145" s="10"/>
       <c r="C145" s="2"/>
       <c r="D145" s="2"/>
       <c r="E145" s="2"/>
@@ -2014,7 +2147,7 @@
     </row>
     <row r="146" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A146" s="2"/>
-      <c r="B146" s="2"/>
+      <c r="B146" s="10"/>
       <c r="C146" s="2"/>
       <c r="D146" s="2"/>
       <c r="E146" s="2"/>
@@ -2023,7 +2156,7 @@
     </row>
     <row r="147" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A147" s="2"/>
-      <c r="B147" s="2"/>
+      <c r="B147" s="10"/>
       <c r="C147" s="2"/>
       <c r="D147" s="2"/>
       <c r="E147" s="2"/>
@@ -2032,7 +2165,7 @@
     </row>
     <row r="148" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A148" s="2"/>
-      <c r="B148" s="2"/>
+      <c r="B148" s="10"/>
       <c r="C148" s="2"/>
       <c r="D148" s="2"/>
       <c r="E148" s="2"/>
@@ -2041,7 +2174,7 @@
     </row>
     <row r="149" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A149" s="2"/>
-      <c r="B149" s="2"/>
+      <c r="B149" s="10"/>
       <c r="C149" s="2"/>
       <c r="D149" s="2"/>
       <c r="E149" s="2"/>
@@ -2050,7 +2183,7 @@
     </row>
     <row r="150" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A150" s="2"/>
-      <c r="B150" s="2"/>
+      <c r="B150" s="10"/>
       <c r="C150" s="2"/>
       <c r="D150" s="2"/>
       <c r="E150" s="2"/>
@@ -2059,7 +2192,7 @@
     </row>
     <row r="151" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A151" s="2"/>
-      <c r="B151" s="2"/>
+      <c r="B151" s="10"/>
       <c r="C151" s="2"/>
       <c r="D151" s="2"/>
       <c r="E151" s="2"/>
@@ -2068,7 +2201,7 @@
     </row>
     <row r="152" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A152" s="2"/>
-      <c r="B152" s="2"/>
+      <c r="B152" s="10"/>
       <c r="C152" s="2"/>
       <c r="D152" s="2"/>
       <c r="E152" s="2"/>
@@ -2077,7 +2210,7 @@
     </row>
     <row r="153" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A153" s="2"/>
-      <c r="B153" s="2"/>
+      <c r="B153" s="10"/>
       <c r="C153" s="2"/>
       <c r="D153" s="2"/>
       <c r="E153" s="2"/>
@@ -2086,7 +2219,7 @@
     </row>
     <row r="154" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A154" s="2"/>
-      <c r="B154" s="2"/>
+      <c r="B154" s="10"/>
       <c r="C154" s="2"/>
       <c r="D154" s="2"/>
       <c r="E154" s="2"/>
@@ -2095,7 +2228,7 @@
     </row>
     <row r="155" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A155" s="2"/>
-      <c r="B155" s="2"/>
+      <c r="B155" s="10"/>
       <c r="C155" s="2"/>
       <c r="D155" s="2"/>
       <c r="E155" s="2"/>
@@ -2104,7 +2237,7 @@
     </row>
     <row r="156" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A156" s="2"/>
-      <c r="B156" s="2"/>
+      <c r="B156" s="10"/>
       <c r="C156" s="2"/>
       <c r="D156" s="2"/>
       <c r="E156" s="2"/>
@@ -2113,7 +2246,7 @@
     </row>
     <row r="157" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A157" s="2"/>
-      <c r="B157" s="2"/>
+      <c r="B157" s="10"/>
       <c r="C157" s="2"/>
       <c r="D157" s="2"/>
       <c r="E157" s="2"/>
@@ -2122,7 +2255,7 @@
     </row>
     <row r="158" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A158" s="2"/>
-      <c r="B158" s="2"/>
+      <c r="B158" s="10"/>
       <c r="C158" s="2"/>
       <c r="D158" s="2"/>
       <c r="E158" s="2"/>
@@ -2131,7 +2264,7 @@
     </row>
     <row r="159" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A159" s="2"/>
-      <c r="B159" s="2"/>
+      <c r="B159" s="10"/>
       <c r="C159" s="2"/>
       <c r="D159" s="2"/>
       <c r="E159" s="2"/>
@@ -2140,7 +2273,7 @@
     </row>
     <row r="160" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A160" s="2"/>
-      <c r="B160" s="2"/>
+      <c r="B160" s="10"/>
       <c r="C160" s="2"/>
       <c r="D160" s="2"/>
       <c r="E160" s="2"/>
@@ -2149,7 +2282,7 @@
     </row>
     <row r="161" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A161" s="2"/>
-      <c r="B161" s="2"/>
+      <c r="B161" s="10"/>
       <c r="C161" s="2"/>
       <c r="D161" s="2"/>
       <c r="E161" s="2"/>
@@ -2158,7 +2291,7 @@
     </row>
     <row r="162" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A162" s="2"/>
-      <c r="B162" s="2"/>
+      <c r="B162" s="10"/>
       <c r="C162" s="2"/>
       <c r="D162" s="2"/>
       <c r="E162" s="2"/>
@@ -2167,7 +2300,7 @@
     </row>
     <row r="163" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A163" s="2"/>
-      <c r="B163" s="2"/>
+      <c r="B163" s="10"/>
       <c r="C163" s="2"/>
       <c r="D163" s="2"/>
       <c r="E163" s="2"/>
@@ -2176,7 +2309,7 @@
     </row>
     <row r="164" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A164" s="2"/>
-      <c r="B164" s="2"/>
+      <c r="B164" s="10"/>
       <c r="C164" s="2"/>
       <c r="D164" s="2"/>
       <c r="E164" s="2"/>
@@ -2185,7 +2318,7 @@
     </row>
     <row r="165" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A165" s="2"/>
-      <c r="B165" s="2"/>
+      <c r="B165" s="10"/>
       <c r="C165" s="2"/>
       <c r="D165" s="2"/>
       <c r="E165" s="2"/>
@@ -2194,7 +2327,7 @@
     </row>
     <row r="166" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A166" s="2"/>
-      <c r="B166" s="2"/>
+      <c r="B166" s="10"/>
       <c r="C166" s="2"/>
       <c r="D166" s="2"/>
       <c r="E166" s="2"/>
@@ -2203,7 +2336,7 @@
     </row>
     <row r="167" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A167" s="2"/>
-      <c r="B167" s="2"/>
+      <c r="B167" s="10"/>
       <c r="C167" s="2"/>
       <c r="D167" s="2"/>
       <c r="E167" s="2"/>
@@ -2212,7 +2345,7 @@
     </row>
     <row r="168" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A168" s="2"/>
-      <c r="B168" s="2"/>
+      <c r="B168" s="10"/>
       <c r="C168" s="2"/>
       <c r="D168" s="2"/>
       <c r="E168" s="2"/>
@@ -2221,7 +2354,7 @@
     </row>
     <row r="169" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A169" s="2"/>
-      <c r="B169" s="2"/>
+      <c r="B169" s="10"/>
       <c r="C169" s="2"/>
       <c r="D169" s="2"/>
       <c r="E169" s="2"/>
@@ -2230,7 +2363,7 @@
     </row>
     <row r="170" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A170" s="2"/>
-      <c r="B170" s="2"/>
+      <c r="B170" s="10"/>
       <c r="C170" s="2"/>
       <c r="D170" s="2"/>
       <c r="E170" s="2"/>
@@ -2239,7 +2372,7 @@
     </row>
     <row r="171" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A171" s="2"/>
-      <c r="B171" s="2"/>
+      <c r="B171" s="10"/>
       <c r="C171" s="2"/>
       <c r="D171" s="2"/>
       <c r="E171" s="2"/>
@@ -2248,7 +2381,7 @@
     </row>
     <row r="172" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A172" s="2"/>
-      <c r="B172" s="2"/>
+      <c r="B172" s="10"/>
       <c r="C172" s="2"/>
       <c r="D172" s="2"/>
       <c r="E172" s="2"/>
@@ -2257,7 +2390,7 @@
     </row>
     <row r="173" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A173" s="2"/>
-      <c r="B173" s="2"/>
+      <c r="B173" s="10"/>
       <c r="C173" s="2"/>
       <c r="D173" s="2"/>
       <c r="E173" s="2"/>
@@ -2266,7 +2399,7 @@
     </row>
     <row r="174" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A174" s="2"/>
-      <c r="B174" s="2"/>
+      <c r="B174" s="10"/>
       <c r="C174" s="2"/>
       <c r="D174" s="2"/>
       <c r="E174" s="2"/>
@@ -2275,7 +2408,7 @@
     </row>
     <row r="175" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A175" s="2"/>
-      <c r="B175" s="2"/>
+      <c r="B175" s="10"/>
       <c r="C175" s="2"/>
       <c r="D175" s="2"/>
       <c r="E175" s="2"/>
@@ -2284,7 +2417,7 @@
     </row>
     <row r="176" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A176" s="2"/>
-      <c r="B176" s="2"/>
+      <c r="B176" s="10"/>
       <c r="C176" s="2"/>
       <c r="D176" s="2"/>
       <c r="E176" s="2"/>
@@ -2293,7 +2426,7 @@
     </row>
     <row r="177" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A177" s="2"/>
-      <c r="B177" s="2"/>
+      <c r="B177" s="10"/>
       <c r="C177" s="2"/>
       <c r="D177" s="2"/>
       <c r="E177" s="2"/>
@@ -2302,7 +2435,7 @@
     </row>
     <row r="178" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A178" s="2"/>
-      <c r="B178" s="2"/>
+      <c r="B178" s="10"/>
       <c r="C178" s="2"/>
       <c r="D178" s="2"/>
       <c r="E178" s="2"/>
@@ -2311,7 +2444,7 @@
     </row>
     <row r="179" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A179" s="2"/>
-      <c r="B179" s="2"/>
+      <c r="B179" s="10"/>
       <c r="C179" s="2"/>
       <c r="D179" s="2"/>
       <c r="E179" s="2"/>
@@ -2320,7 +2453,7 @@
     </row>
     <row r="180" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A180" s="2"/>
-      <c r="B180" s="2"/>
+      <c r="B180" s="10"/>
       <c r="C180" s="2"/>
       <c r="D180" s="2"/>
       <c r="E180" s="2"/>
@@ -2329,7 +2462,7 @@
     </row>
     <row r="181" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A181" s="2"/>
-      <c r="B181" s="2"/>
+      <c r="B181" s="10"/>
       <c r="C181" s="2"/>
       <c r="D181" s="2"/>
       <c r="E181" s="2"/>
@@ -2338,7 +2471,7 @@
     </row>
     <row r="182" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A182" s="2"/>
-      <c r="B182" s="2"/>
+      <c r="B182" s="10"/>
       <c r="C182" s="2"/>
       <c r="D182" s="2"/>
       <c r="E182" s="2"/>
@@ -2347,7 +2480,7 @@
     </row>
     <row r="183" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A183" s="2"/>
-      <c r="B183" s="2"/>
+      <c r="B183" s="10"/>
       <c r="C183" s="2"/>
       <c r="D183" s="2"/>
       <c r="E183" s="2"/>
@@ -2356,7 +2489,7 @@
     </row>
     <row r="184" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A184" s="2"/>
-      <c r="B184" s="2"/>
+      <c r="B184" s="10"/>
       <c r="C184" s="2"/>
       <c r="D184" s="2"/>
       <c r="E184" s="2"/>
@@ -2365,7 +2498,7 @@
     </row>
     <row r="185" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A185" s="2"/>
-      <c r="B185" s="2"/>
+      <c r="B185" s="10"/>
       <c r="C185" s="2"/>
       <c r="D185" s="2"/>
       <c r="E185" s="2"/>
@@ -2374,7 +2507,7 @@
     </row>
     <row r="186" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A186" s="2"/>
-      <c r="B186" s="2"/>
+      <c r="B186" s="10"/>
       <c r="C186" s="2"/>
       <c r="D186" s="2"/>
       <c r="E186" s="2"/>
@@ -2383,7 +2516,7 @@
     </row>
     <row r="187" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A187" s="2"/>
-      <c r="B187" s="2"/>
+      <c r="B187" s="10"/>
       <c r="C187" s="2"/>
       <c r="D187" s="2"/>
       <c r="E187" s="2"/>
@@ -2392,7 +2525,7 @@
     </row>
     <row r="188" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A188" s="2"/>
-      <c r="B188" s="2"/>
+      <c r="B188" s="10"/>
       <c r="C188" s="2"/>
       <c r="D188" s="2"/>
       <c r="E188" s="2"/>
@@ -2401,7 +2534,7 @@
     </row>
     <row r="189" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A189" s="2"/>
-      <c r="B189" s="2"/>
+      <c r="B189" s="10"/>
       <c r="C189" s="2"/>
       <c r="D189" s="2"/>
       <c r="E189" s="2"/>
@@ -2410,7 +2543,7 @@
     </row>
     <row r="190" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A190" s="2"/>
-      <c r="B190" s="2"/>
+      <c r="B190" s="10"/>
       <c r="C190" s="2"/>
       <c r="D190" s="2"/>
       <c r="E190" s="2"/>
@@ -2419,7 +2552,7 @@
     </row>
     <row r="191" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A191" s="2"/>
-      <c r="B191" s="2"/>
+      <c r="B191" s="10"/>
       <c r="C191" s="2"/>
       <c r="D191" s="2"/>
       <c r="E191" s="2"/>
@@ -2428,7 +2561,7 @@
     </row>
     <row r="192" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A192" s="2"/>
-      <c r="B192" s="2"/>
+      <c r="B192" s="10"/>
       <c r="C192" s="2"/>
       <c r="D192" s="2"/>
       <c r="E192" s="2"/>
@@ -2437,7 +2570,7 @@
     </row>
     <row r="193" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A193" s="2"/>
-      <c r="B193" s="2"/>
+      <c r="B193" s="10"/>
       <c r="C193" s="2"/>
       <c r="D193" s="2"/>
       <c r="E193" s="2"/>
@@ -2446,7 +2579,7 @@
     </row>
     <row r="194" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A194" s="2"/>
-      <c r="B194" s="2"/>
+      <c r="B194" s="10"/>
       <c r="C194" s="2"/>
       <c r="D194" s="2"/>
       <c r="E194" s="2"/>
@@ -2455,7 +2588,7 @@
     </row>
     <row r="195" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A195" s="2"/>
-      <c r="B195" s="2"/>
+      <c r="B195" s="10"/>
       <c r="C195" s="2"/>
       <c r="D195" s="2"/>
       <c r="E195" s="2"/>
@@ -2464,7 +2597,7 @@
     </row>
     <row r="196" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A196" s="2"/>
-      <c r="B196" s="2"/>
+      <c r="B196" s="10"/>
       <c r="C196" s="2"/>
       <c r="D196" s="2"/>
       <c r="E196" s="2"/>
@@ -2473,7 +2606,7 @@
     </row>
     <row r="197" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A197" s="2"/>
-      <c r="B197" s="2"/>
+      <c r="B197" s="10"/>
       <c r="C197" s="2"/>
       <c r="D197" s="2"/>
       <c r="E197" s="2"/>
@@ -2482,7 +2615,7 @@
     </row>
     <row r="198" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A198" s="2"/>
-      <c r="B198" s="2"/>
+      <c r="B198" s="10"/>
       <c r="C198" s="2"/>
       <c r="D198" s="2"/>
       <c r="E198" s="2"/>
@@ -2491,7 +2624,7 @@
     </row>
     <row r="199" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A199" s="2"/>
-      <c r="B199" s="2"/>
+      <c r="B199" s="10"/>
       <c r="C199" s="2"/>
       <c r="D199" s="2"/>
       <c r="E199" s="2"/>
@@ -2500,7 +2633,7 @@
     </row>
     <row r="200" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A200" s="2"/>
-      <c r="B200" s="2"/>
+      <c r="B200" s="10"/>
       <c r="C200" s="2"/>
       <c r="D200" s="2"/>
       <c r="E200" s="2"/>
@@ -2509,7 +2642,7 @@
     </row>
     <row r="201" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A201" s="2"/>
-      <c r="B201" s="2"/>
+      <c r="B201" s="10"/>
       <c r="C201" s="2"/>
       <c r="D201" s="2"/>
       <c r="E201" s="2"/>
@@ -2518,7 +2651,7 @@
     </row>
     <row r="202" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A202" s="2"/>
-      <c r="B202" s="2"/>
+      <c r="B202" s="10"/>
       <c r="C202" s="2"/>
       <c r="D202" s="2"/>
       <c r="E202" s="2"/>
@@ -2527,7 +2660,7 @@
     </row>
     <row r="203" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A203" s="2"/>
-      <c r="B203" s="2"/>
+      <c r="B203" s="10"/>
       <c r="C203" s="2"/>
       <c r="D203" s="2"/>
       <c r="E203" s="2"/>
@@ -2536,7 +2669,7 @@
     </row>
     <row r="204" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A204" s="2"/>
-      <c r="B204" s="2"/>
+      <c r="B204" s="10"/>
       <c r="C204" s="2"/>
       <c r="D204" s="2"/>
       <c r="E204" s="2"/>
@@ -2545,7 +2678,7 @@
     </row>
     <row r="205" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A205" s="2"/>
-      <c r="B205" s="2"/>
+      <c r="B205" s="10"/>
       <c r="C205" s="2"/>
       <c r="D205" s="2"/>
       <c r="E205" s="2"/>
@@ -2554,7 +2687,7 @@
     </row>
     <row r="206" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A206" s="2"/>
-      <c r="B206" s="2"/>
+      <c r="B206" s="10"/>
       <c r="C206" s="2"/>
       <c r="D206" s="2"/>
       <c r="E206" s="2"/>
@@ -2563,7 +2696,7 @@
     </row>
     <row r="207" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A207" s="2"/>
-      <c r="B207" s="2"/>
+      <c r="B207" s="10"/>
       <c r="C207" s="2"/>
       <c r="D207" s="2"/>
       <c r="E207" s="2"/>
@@ -2572,7 +2705,7 @@
     </row>
     <row r="208" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A208" s="2"/>
-      <c r="B208" s="2"/>
+      <c r="B208" s="10"/>
       <c r="C208" s="2"/>
       <c r="D208" s="2"/>
       <c r="E208" s="2"/>
@@ -2581,7 +2714,7 @@
     </row>
     <row r="209" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A209" s="2"/>
-      <c r="B209" s="2"/>
+      <c r="B209" s="10"/>
       <c r="C209" s="2"/>
       <c r="D209" s="2"/>
       <c r="E209" s="2"/>
@@ -2590,7 +2723,7 @@
     </row>
     <row r="210" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A210" s="2"/>
-      <c r="B210" s="2"/>
+      <c r="B210" s="10"/>
       <c r="C210" s="2"/>
       <c r="D210" s="2"/>
       <c r="E210" s="2"/>
@@ -2599,7 +2732,7 @@
     </row>
     <row r="211" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A211" s="2"/>
-      <c r="B211" s="2"/>
+      <c r="B211" s="10"/>
       <c r="C211" s="2"/>
       <c r="D211" s="2"/>
       <c r="E211" s="2"/>
@@ -2608,7 +2741,7 @@
     </row>
     <row r="212" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A212" s="2"/>
-      <c r="B212" s="2"/>
+      <c r="B212" s="10"/>
       <c r="C212" s="2"/>
       <c r="D212" s="2"/>
       <c r="E212" s="2"/>
@@ -2617,7 +2750,7 @@
     </row>
     <row r="213" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A213" s="2"/>
-      <c r="B213" s="2"/>
+      <c r="B213" s="10"/>
       <c r="C213" s="2"/>
       <c r="D213" s="2"/>
       <c r="E213" s="2"/>
@@ -2626,7 +2759,7 @@
     </row>
     <row r="214" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A214" s="2"/>
-      <c r="B214" s="2"/>
+      <c r="B214" s="10"/>
       <c r="C214" s="2"/>
       <c r="D214" s="2"/>
       <c r="E214" s="2"/>
@@ -2635,7 +2768,7 @@
     </row>
     <row r="215" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A215" s="2"/>
-      <c r="B215" s="2"/>
+      <c r="B215" s="10"/>
       <c r="C215" s="2"/>
       <c r="D215" s="2"/>
       <c r="E215" s="2"/>
@@ -2644,7 +2777,7 @@
     </row>
     <row r="216" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A216" s="2"/>
-      <c r="B216" s="2"/>
+      <c r="B216" s="10"/>
       <c r="C216" s="2"/>
       <c r="D216" s="2"/>
       <c r="E216" s="2"/>
@@ -2653,7 +2786,7 @@
     </row>
     <row r="217" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A217" s="2"/>
-      <c r="B217" s="2"/>
+      <c r="B217" s="10"/>
       <c r="C217" s="2"/>
       <c r="D217" s="2"/>
       <c r="E217" s="2"/>
@@ -2662,7 +2795,7 @@
     </row>
     <row r="218" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A218" s="2"/>
-      <c r="B218" s="2"/>
+      <c r="B218" s="10"/>
       <c r="C218" s="2"/>
       <c r="D218" s="2"/>
       <c r="E218" s="2"/>
@@ -2671,7 +2804,7 @@
     </row>
     <row r="219" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A219" s="2"/>
-      <c r="B219" s="2"/>
+      <c r="B219" s="10"/>
       <c r="C219" s="2"/>
       <c r="D219" s="2"/>
       <c r="E219" s="2"/>
@@ -2680,7 +2813,7 @@
     </row>
     <row r="220" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A220" s="2"/>
-      <c r="B220" s="2"/>
+      <c r="B220" s="10"/>
       <c r="C220" s="2"/>
       <c r="D220" s="2"/>
       <c r="E220" s="2"/>
@@ -2689,7 +2822,7 @@
     </row>
     <row r="221" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A221" s="2"/>
-      <c r="B221" s="2"/>
+      <c r="B221" s="10"/>
       <c r="C221" s="2"/>
       <c r="D221" s="2"/>
       <c r="E221" s="2"/>
@@ -2698,7 +2831,7 @@
     </row>
     <row r="222" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A222" s="2"/>
-      <c r="B222" s="2"/>
+      <c r="B222" s="10"/>
       <c r="C222" s="2"/>
       <c r="D222" s="2"/>
       <c r="E222" s="2"/>
@@ -2707,7 +2840,7 @@
     </row>
     <row r="223" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A223" s="2"/>
-      <c r="B223" s="2"/>
+      <c r="B223" s="10"/>
       <c r="C223" s="2"/>
       <c r="D223" s="2"/>
       <c r="E223" s="2"/>
@@ -2716,7 +2849,7 @@
     </row>
     <row r="224" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A224" s="2"/>
-      <c r="B224" s="2"/>
+      <c r="B224" s="10"/>
       <c r="C224" s="2"/>
       <c r="D224" s="2"/>
       <c r="E224" s="2"/>
@@ -2725,7 +2858,7 @@
     </row>
     <row r="225" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A225" s="2"/>
-      <c r="B225" s="2"/>
+      <c r="B225" s="10"/>
       <c r="C225" s="2"/>
       <c r="D225" s="2"/>
       <c r="E225" s="2"/>
@@ -2734,7 +2867,7 @@
     </row>
     <row r="226" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A226" s="2"/>
-      <c r="B226" s="2"/>
+      <c r="B226" s="10"/>
       <c r="C226" s="2"/>
       <c r="D226" s="2"/>
       <c r="E226" s="2"/>
@@ -2743,7 +2876,7 @@
     </row>
     <row r="227" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A227" s="2"/>
-      <c r="B227" s="2"/>
+      <c r="B227" s="10"/>
       <c r="C227" s="2"/>
       <c r="D227" s="2"/>
       <c r="E227" s="2"/>
@@ -2752,7 +2885,7 @@
     </row>
     <row r="228" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A228" s="2"/>
-      <c r="B228" s="2"/>
+      <c r="B228" s="10"/>
       <c r="C228" s="2"/>
       <c r="D228" s="2"/>
       <c r="E228" s="2"/>
@@ -2761,7 +2894,7 @@
     </row>
     <row r="229" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A229" s="2"/>
-      <c r="B229" s="2"/>
+      <c r="B229" s="10"/>
       <c r="C229" s="2"/>
       <c r="D229" s="2"/>
       <c r="E229" s="2"/>
@@ -2770,7 +2903,7 @@
     </row>
     <row r="230" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A230" s="2"/>
-      <c r="B230" s="2"/>
+      <c r="B230" s="10"/>
       <c r="C230" s="2"/>
       <c r="D230" s="2"/>
       <c r="E230" s="2"/>
@@ -2779,7 +2912,7 @@
     </row>
     <row r="231" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A231" s="2"/>
-      <c r="B231" s="2"/>
+      <c r="B231" s="10"/>
       <c r="C231" s="2"/>
       <c r="D231" s="2"/>
       <c r="E231" s="2"/>
@@ -2788,7 +2921,7 @@
     </row>
     <row r="232" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A232" s="2"/>
-      <c r="B232" s="2"/>
+      <c r="B232" s="10"/>
       <c r="C232" s="2"/>
       <c r="D232" s="2"/>
       <c r="E232" s="2"/>
@@ -2797,7 +2930,7 @@
     </row>
     <row r="233" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A233" s="2"/>
-      <c r="B233" s="2"/>
+      <c r="B233" s="10"/>
       <c r="C233" s="2"/>
       <c r="D233" s="2"/>
       <c r="E233" s="2"/>
@@ -2806,7 +2939,7 @@
     </row>
     <row r="234" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A234" s="2"/>
-      <c r="B234" s="2"/>
+      <c r="B234" s="10"/>
       <c r="C234" s="2"/>
       <c r="D234" s="2"/>
       <c r="E234" s="2"/>
@@ -2815,7 +2948,7 @@
     </row>
     <row r="235" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A235" s="2"/>
-      <c r="B235" s="2"/>
+      <c r="B235" s="10"/>
       <c r="C235" s="2"/>
       <c r="D235" s="2"/>
       <c r="E235" s="2"/>
@@ -2824,7 +2957,7 @@
     </row>
     <row r="236" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A236" s="2"/>
-      <c r="B236" s="2"/>
+      <c r="B236" s="10"/>
       <c r="C236" s="2"/>
       <c r="D236" s="2"/>
       <c r="E236" s="2"/>
@@ -2833,7 +2966,7 @@
     </row>
     <row r="237" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A237" s="2"/>
-      <c r="B237" s="2"/>
+      <c r="B237" s="10"/>
       <c r="C237" s="2"/>
       <c r="D237" s="2"/>
       <c r="E237" s="2"/>
@@ -2842,7 +2975,7 @@
     </row>
     <row r="238" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A238" s="2"/>
-      <c r="B238" s="2"/>
+      <c r="B238" s="10"/>
       <c r="C238" s="2"/>
       <c r="D238" s="2"/>
       <c r="E238" s="2"/>
@@ -2851,7 +2984,7 @@
     </row>
     <row r="239" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A239" s="2"/>
-      <c r="B239" s="2"/>
+      <c r="B239" s="10"/>
       <c r="C239" s="2"/>
       <c r="D239" s="2"/>
       <c r="E239" s="2"/>
@@ -2860,7 +2993,7 @@
     </row>
     <row r="240" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A240" s="2"/>
-      <c r="B240" s="2"/>
+      <c r="B240" s="10"/>
       <c r="C240" s="2"/>
       <c r="D240" s="2"/>
       <c r="E240" s="2"/>
@@ -2869,7 +3002,7 @@
     </row>
     <row r="241" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A241" s="2"/>
-      <c r="B241" s="2"/>
+      <c r="B241" s="10"/>
       <c r="C241" s="2"/>
       <c r="D241" s="2"/>
       <c r="E241" s="2"/>
@@ -2878,7 +3011,7 @@
     </row>
     <row r="242" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A242" s="2"/>
-      <c r="B242" s="2"/>
+      <c r="B242" s="10"/>
       <c r="C242" s="2"/>
       <c r="D242" s="2"/>
       <c r="E242" s="2"/>
@@ -2887,7 +3020,7 @@
     </row>
     <row r="243" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A243" s="2"/>
-      <c r="B243" s="2"/>
+      <c r="B243" s="10"/>
       <c r="C243" s="2"/>
       <c r="D243" s="2"/>
       <c r="E243" s="2"/>
@@ -2896,7 +3029,7 @@
     </row>
     <row r="244" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A244" s="2"/>
-      <c r="B244" s="2"/>
+      <c r="B244" s="10"/>
       <c r="C244" s="2"/>
       <c r="D244" s="2"/>
       <c r="E244" s="2"/>
@@ -2905,7 +3038,7 @@
     </row>
     <row r="245" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A245" s="2"/>
-      <c r="B245" s="2"/>
+      <c r="B245" s="10"/>
       <c r="C245" s="2"/>
       <c r="D245" s="2"/>
       <c r="E245" s="2"/>
@@ -2914,7 +3047,7 @@
     </row>
     <row r="246" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A246" s="2"/>
-      <c r="B246" s="2"/>
+      <c r="B246" s="10"/>
       <c r="C246" s="2"/>
       <c r="D246" s="2"/>
       <c r="E246" s="2"/>
@@ -2923,7 +3056,7 @@
     </row>
     <row r="247" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A247" s="2"/>
-      <c r="B247" s="2"/>
+      <c r="B247" s="10"/>
       <c r="C247" s="2"/>
       <c r="D247" s="2"/>
       <c r="E247" s="2"/>
@@ -2932,7 +3065,7 @@
     </row>
     <row r="248" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A248" s="2"/>
-      <c r="B248" s="2"/>
+      <c r="B248" s="10"/>
       <c r="C248" s="2"/>
       <c r="D248" s="2"/>
       <c r="E248" s="2"/>
@@ -2941,7 +3074,7 @@
     </row>
     <row r="249" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A249" s="2"/>
-      <c r="B249" s="2"/>
+      <c r="B249" s="10"/>
       <c r="C249" s="2"/>
       <c r="D249" s="2"/>
       <c r="E249" s="2"/>
@@ -2950,7 +3083,7 @@
     </row>
     <row r="250" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A250" s="2"/>
-      <c r="B250" s="2"/>
+      <c r="B250" s="10"/>
       <c r="C250" s="2"/>
       <c r="D250" s="2"/>
       <c r="E250" s="2"/>
@@ -2959,7 +3092,7 @@
     </row>
     <row r="251" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A251" s="2"/>
-      <c r="B251" s="2"/>
+      <c r="B251" s="10"/>
       <c r="C251" s="2"/>
       <c r="D251" s="2"/>
       <c r="E251" s="2"/>
@@ -2968,7 +3101,7 @@
     </row>
     <row r="252" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A252" s="2"/>
-      <c r="B252" s="2"/>
+      <c r="B252" s="10"/>
       <c r="C252" s="2"/>
       <c r="D252" s="2"/>
       <c r="E252" s="2"/>
@@ -2977,7 +3110,7 @@
     </row>
     <row r="253" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A253" s="2"/>
-      <c r="B253" s="2"/>
+      <c r="B253" s="10"/>
       <c r="C253" s="2"/>
       <c r="D253" s="2"/>
       <c r="E253" s="2"/>
@@ -2986,7 +3119,7 @@
     </row>
     <row r="254" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A254" s="2"/>
-      <c r="B254" s="2"/>
+      <c r="B254" s="10"/>
       <c r="C254" s="2"/>
       <c r="D254" s="2"/>
       <c r="E254" s="2"/>
@@ -2995,7 +3128,7 @@
     </row>
     <row r="255" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A255" s="2"/>
-      <c r="B255" s="2"/>
+      <c r="B255" s="10"/>
       <c r="C255" s="2"/>
       <c r="D255" s="2"/>
       <c r="E255" s="2"/>
@@ -3004,7 +3137,7 @@
     </row>
     <row r="256" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A256" s="2"/>
-      <c r="B256" s="2"/>
+      <c r="B256" s="10"/>
       <c r="C256" s="2"/>
       <c r="D256" s="2"/>
       <c r="E256" s="2"/>
@@ -3013,7 +3146,7 @@
     </row>
     <row r="257" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A257" s="2"/>
-      <c r="B257" s="2"/>
+      <c r="B257" s="10"/>
       <c r="C257" s="2"/>
       <c r="D257" s="2"/>
       <c r="E257" s="2"/>
@@ -3022,7 +3155,7 @@
     </row>
     <row r="258" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A258" s="2"/>
-      <c r="B258" s="2"/>
+      <c r="B258" s="10"/>
       <c r="C258" s="2"/>
       <c r="D258" s="2"/>
       <c r="E258" s="2"/>
@@ -3031,7 +3164,7 @@
     </row>
     <row r="259" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A259" s="2"/>
-      <c r="B259" s="2"/>
+      <c r="B259" s="10"/>
       <c r="C259" s="2"/>
       <c r="D259" s="2"/>
       <c r="E259" s="2"/>
@@ -3040,7 +3173,7 @@
     </row>
     <row r="260" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A260" s="2"/>
-      <c r="B260" s="2"/>
+      <c r="B260" s="10"/>
       <c r="C260" s="2"/>
       <c r="D260" s="2"/>
       <c r="E260" s="2"/>
@@ -3049,7 +3182,7 @@
     </row>
     <row r="261" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A261" s="2"/>
-      <c r="B261" s="2"/>
+      <c r="B261" s="10"/>
       <c r="C261" s="2"/>
       <c r="D261" s="2"/>
       <c r="E261" s="2"/>
@@ -3058,7 +3191,7 @@
     </row>
     <row r="262" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A262" s="2"/>
-      <c r="B262" s="2"/>
+      <c r="B262" s="10"/>
       <c r="C262" s="2"/>
       <c r="D262" s="2"/>
       <c r="E262" s="2"/>
@@ -3067,7 +3200,7 @@
     </row>
     <row r="263" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A263" s="2"/>
-      <c r="B263" s="2"/>
+      <c r="B263" s="10"/>
       <c r="C263" s="2"/>
       <c r="D263" s="2"/>
       <c r="E263" s="2"/>
@@ -3076,7 +3209,7 @@
     </row>
     <row r="264" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A264" s="2"/>
-      <c r="B264" s="2"/>
+      <c r="B264" s="10"/>
       <c r="C264" s="2"/>
       <c r="D264" s="2"/>
       <c r="E264" s="2"/>
@@ -3085,7 +3218,7 @@
     </row>
     <row r="265" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A265" s="2"/>
-      <c r="B265" s="2"/>
+      <c r="B265" s="10"/>
       <c r="C265" s="2"/>
       <c r="D265" s="2"/>
       <c r="E265" s="2"/>
@@ -3094,7 +3227,7 @@
     </row>
     <row r="266" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A266" s="2"/>
-      <c r="B266" s="2"/>
+      <c r="B266" s="10"/>
       <c r="C266" s="2"/>
       <c r="D266" s="2"/>
       <c r="E266" s="2"/>
@@ -3103,7 +3236,7 @@
     </row>
     <row r="267" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A267" s="2"/>
-      <c r="B267" s="2"/>
+      <c r="B267" s="10"/>
       <c r="C267" s="2"/>
       <c r="D267" s="2"/>
       <c r="E267" s="2"/>
@@ -3112,7 +3245,7 @@
     </row>
     <row r="268" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A268" s="2"/>
-      <c r="B268" s="2"/>
+      <c r="B268" s="10"/>
       <c r="C268" s="2"/>
       <c r="D268" s="2"/>
       <c r="E268" s="2"/>
@@ -3121,7 +3254,7 @@
     </row>
     <row r="269" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A269" s="2"/>
-      <c r="B269" s="2"/>
+      <c r="B269" s="10"/>
       <c r="C269" s="2"/>
       <c r="D269" s="2"/>
       <c r="E269" s="2"/>
@@ -3130,7 +3263,7 @@
     </row>
     <row r="270" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A270" s="2"/>
-      <c r="B270" s="2"/>
+      <c r="B270" s="10"/>
       <c r="C270" s="2"/>
       <c r="D270" s="2"/>
       <c r="E270" s="2"/>
@@ -3139,7 +3272,7 @@
     </row>
     <row r="271" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A271" s="2"/>
-      <c r="B271" s="2"/>
+      <c r="B271" s="10"/>
       <c r="C271" s="2"/>
       <c r="D271" s="2"/>
       <c r="E271" s="2"/>
@@ -3148,7 +3281,7 @@
     </row>
     <row r="272" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A272" s="2"/>
-      <c r="B272" s="2"/>
+      <c r="B272" s="10"/>
       <c r="C272" s="2"/>
       <c r="D272" s="2"/>
       <c r="E272" s="2"/>
@@ -3157,7 +3290,7 @@
     </row>
     <row r="273" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A273" s="2"/>
-      <c r="B273" s="2"/>
+      <c r="B273" s="10"/>
       <c r="C273" s="2"/>
       <c r="D273" s="2"/>
       <c r="E273" s="2"/>
@@ -3166,7 +3299,7 @@
     </row>
     <row r="274" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A274" s="2"/>
-      <c r="B274" s="2"/>
+      <c r="B274" s="10"/>
       <c r="C274" s="2"/>
       <c r="D274" s="2"/>
       <c r="E274" s="2"/>
@@ -3176,6 +3309,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G4" r:id="rId1"/>
+    <hyperlink ref="G9" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Update: Added more excel entries. Renaming fixes.
</commit_message>
<xml_diff>
--- a/All Other Data/s2cAllRawDataExcel.xlsx
+++ b/All Other Data/s2cAllRawDataExcel.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="74">
   <si>
     <t>Name</t>
   </si>
@@ -99,9 +99,6 @@
   </si>
   <si>
     <t>Muhammad</t>
-  </si>
-  <si>
-    <t>Losing parents at early age</t>
   </si>
   <si>
     <t>Jesus Christ</t>
@@ -158,10 +155,6 @@
     <t>http://www.famoushomeschoolers.net/bio_einstein.html#.WGLgw7YrLBI</t>
   </si>
   <si>
-    <t>Einstein’s parents wanted him to pursue a career in electrical engineering. Without a high school diploma, Einstein applied to the Polytechnic Institute at Zurich, Switzerland. He failed the entrance examination although he got exceptional marks in the mathematics and physics sections. Einstein described himself as “a conscientious but unassuming young man who had acquired his meagre store of pertinent knowledge of the essentials through self study. 
-He basically taught himself math and physics through books and self-study and skipped lectures and stopped going to classes that didn't interest him</t>
-  </si>
-  <si>
     <t>Slow Learner, Late Bloomer, Possible Asperger's Syndrome, Unsociableness, Rejected from Entrance Exam</t>
   </si>
   <si>
@@ -262,6 +255,26 @@
   </si>
   <si>
     <t>Canaan</t>
+  </si>
+  <si>
+    <t>The ink of the scholar is more sacred than the blood of the martyr.
+Four things support the world: the learning of the wise, the justice of the great, the prayers of the good, and the valor of the brave
+To overcome evil with good is good, to resist evil by evil is evil.
+None of you truly believes until he wishes for his brother what he wishes for himself.
+Kindness is a mark of faith, and whoever has not kindness has not faith.</t>
+  </si>
+  <si>
+    <t>Orphaned, Depression, Suicidal Thoughts, Death of Spouse, Persecution</t>
+  </si>
+  <si>
+    <t>4/20/571</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lost his parents at an early age. Was brought up by his grandparents. Became a prophet at 40 and started his preaching although nobody listened in the beginning. He was said to have gone through deep depression and suicidal thoughts while receiving his revelations. After he gained his following, he was persecuted and fled to Ethiopia. He also lost his wife and uncle during this period. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Einstein’s parents wanted him to pursue a career in electrical engineering. Without a high school diploma, Einstein applied to the Polytechnic Institute at Zurich, Switzerland. He failed the entrance examination although he got exceptional marks in the mathematics and physics sections. Einstein described himself as “a conscientious but unassuming young man who had acquired his meagre store of pertinent knowledge of the essentials through self study. 
+He basically taught himself math and physics through books and self-study and skipped lectures and stopped going to classes that didn't interest him. When he was working on the Theory of Relativity, he was working as an Assistant Examiner at a patent office. </t>
   </si>
 </sst>
 </file>
@@ -673,8 +686,8 @@
   <dimension ref="A1:G274"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -728,7 +741,7 @@
         <v>10</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>9</v>
@@ -745,13 +758,13 @@
         <v>17</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G3" s="2"/>
     </row>
@@ -760,36 +773,36 @@
         <v>15</v>
       </c>
       <c r="B4" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="8" t="s">
         <v>31</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="372" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>18</v>
@@ -802,13 +815,13 @@
         <v>19</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -825,7 +838,7 @@
         <v>22</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>23</v>
@@ -833,96 +846,102 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="93" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="409" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="10"/>
+      <c r="B8" s="10" t="s">
+        <v>71</v>
+      </c>
       <c r="C8" s="2" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+        <v>59</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="409" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B9" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="409" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="C10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="248" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" ht="93" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -930,13 +949,13 @@
     </row>
     <row r="13" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="10" t="s">
-        <v>48</v>
-      </c>
       <c r="C13" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -945,11 +964,11 @@
     </row>
     <row r="14" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B14" s="10"/>
       <c r="C14" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -958,11 +977,11 @@
     </row>
     <row r="15" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -971,13 +990,13 @@
     </row>
     <row r="16" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B16" s="10">
         <v>15662</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>

</xml_diff>

<commit_message>
Update: Added Ogilvy and Santiago Ramon y Cajal to list, etc
</commit_message>
<xml_diff>
--- a/All Other Data/s2cAllRawDataExcel.xlsx
+++ b/All Other Data/s2cAllRawDataExcel.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="84">
   <si>
     <t>Name</t>
   </si>
@@ -276,12 +276,50 @@
     <t xml:space="preserve">Einstein’s parents wanted him to pursue a career in electrical engineering. Without a high school diploma, Einstein applied to the Polytechnic Institute at Zurich, Switzerland. He failed the entrance examination although he got exceptional marks in the mathematics and physics sections. Einstein described himself as “a conscientious but unassuming young man who had acquired his meagre store of pertinent knowledge of the essentials through self study. 
 He basically taught himself math and physics through books and self-study and skipped lectures and stopped going to classes that didn't interest him. When he was working on the Theory of Relativity, he was working as an Assistant Examiner at a patent office. </t>
   </si>
+  <si>
+    <t>Santiago Ramón y Cajal</t>
+  </si>
+  <si>
+    <t>Also known as the father of neuroscience, Santiago Ramon y Cajal was a juvenile delinquent and a late bloomer. He said he interacted with people much smarter than he but they all suffered from biases and carelessness. He said his own success was due to perseverance, not genius.</t>
+  </si>
+  <si>
+    <t>5/1/1852</t>
+  </si>
+  <si>
+    <t>Late Bloomer</t>
+  </si>
+  <si>
+    <t>The Wrights Brothers</t>
+  </si>
+  <si>
+    <t>No Formal Education</t>
+  </si>
+  <si>
+    <t>Langley was their rival well-connected and all the financial resources. They were poor, no connections, uneducated. But they were inspired and motivated by changing the world.</t>
+  </si>
+  <si>
+    <t>When we think what we might have accomplished if we had been able to devote this time to experiments, we feel very sad, but it is always easier to deal with things than with men, and no one can direct his life entirely as he would choose. Wilbur Wright</t>
+  </si>
+  <si>
+    <t>http://www.azquotes.com/</t>
+  </si>
+  <si>
+    <t>Every man if he so desires becomes scultor of his own brain. 
+All great work is the fruit of patience and perseverance, combined with tenacious concentration on a subject over a period of months or years.
+To know the brain is equivalent to ascertaining the material course of thought and will, to discovering the intimate history of life in its perpetual duel with  external forces
+It is idle to dispute with old men. Their opinions, like their cranial sutures, are ossified.
+I would be the last to deny that the greatest scientific pioneers belonged to an aristocracy of the spirit and were exceptionally intelligent, something that we as modest investigators will never attain, no matter how much we exert ourselves. Nevertheless … I continue to believe that there is always room for anyone with average intelligence … to utilize his energy and … any man could, if he were so inclined, be the sculptor of his own brain, and that even the least gifted may, like the poorest land that has been well-cultivated and fertilized, produce an abundant harvest.
+It is notorious that the desire to live increases as life itself shortens.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
+  </numFmts>
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -328,6 +366,12 @@
       <color rgb="FF000000"/>
       <name val="Times"/>
     </font>
+    <font>
+      <sz val="21.6"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -371,7 +415,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -398,13 +442,30 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -686,29 +747,31 @@
   <dimension ref="A1:G274"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F17" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="48.1640625" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" style="12" customWidth="1"/>
-    <col min="3" max="3" width="34" customWidth="1"/>
+    <col min="1" max="1" width="48.1640625" style="14" customWidth="1"/>
+    <col min="2" max="2" width="28" style="17" customWidth="1"/>
+    <col min="3" max="3" width="34" style="12" customWidth="1"/>
     <col min="4" max="4" width="21.33203125" customWidth="1"/>
-    <col min="5" max="5" width="67.5" customWidth="1"/>
+    <col min="5" max="5" width="100.33203125" customWidth="1"/>
     <col min="6" max="6" width="47.33203125" customWidth="1"/>
     <col min="7" max="7" width="46.6640625" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -725,13 +788,13 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="3" customFormat="1" ht="291" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -748,13 +811,13 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="409.6" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="11" t="s">
         <v>17</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -769,13 +832,13 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" ht="409" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="11" t="s">
         <v>41</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -791,14 +854,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="372" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:7" ht="248" x14ac:dyDescent="0.35">
+      <c r="A5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="11" t="s">
         <v>64</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -811,13 +874,13 @@
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="62" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="11" t="s">
         <v>20</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -828,13 +891,13 @@
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="62" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="15">
         <v>10608</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="11" t="s">
         <v>22</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -847,13 +910,13 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" ht="409" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="11" t="s">
         <v>70</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -868,13 +931,13 @@
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="409" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="11" t="s">
         <v>65</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -889,13 +952,13 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="409" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="11" t="s">
         <v>37</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -912,13 +975,13 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="248" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="11" t="s">
         <v>20</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -931,13 +994,13 @@
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" ht="93" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="11" t="s">
         <v>43</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -948,13 +1011,13 @@
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="11" t="s">
         <v>45</v>
       </c>
       <c r="D13" s="2"/>
@@ -963,11 +1026,11 @@
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="2" t="s">
+      <c r="B14" s="15"/>
+      <c r="C14" s="11" t="s">
         <v>45</v>
       </c>
       <c r="D14" s="2"/>
@@ -976,11 +1039,11 @@
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="2" t="s">
+      <c r="B15" s="15"/>
+      <c r="C15" s="11" t="s">
         <v>49</v>
       </c>
       <c r="D15" s="2"/>
@@ -989,13 +1052,13 @@
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="10">
+      <c r="B16" s="15">
         <v>15662</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="11" t="s">
         <v>45</v>
       </c>
       <c r="D16" s="2"/>
@@ -1003,2323 +1066,2343 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A17" s="2"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="2"/>
+    <row r="17" spans="1:7" ht="409" x14ac:dyDescent="0.35">
+      <c r="A17" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>77</v>
+      </c>
       <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A18" s="2"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="2"/>
+      <c r="E17" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="310" x14ac:dyDescent="0.35">
+      <c r="A18" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" s="15"/>
+      <c r="C18" s="11" t="s">
+        <v>79</v>
+      </c>
       <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
+      <c r="E18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A19" s="2"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="2"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="11"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A20" s="2"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="2"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="11"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A21" s="2"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="2"/>
+      <c r="A21" s="11"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="11"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A22" s="2"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="2"/>
+      <c r="A22" s="11"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="11"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
     <row r="23" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A23" s="2"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="2"/>
+      <c r="A23" s="11"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="11"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
     <row r="24" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A24" s="2"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="2"/>
+      <c r="A24" s="11"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="11"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
     <row r="25" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A25" s="2"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="2"/>
+      <c r="A25" s="11"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="11"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A26" s="2"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="2"/>
+      <c r="A26" s="11"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="11"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A27" s="2"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="2"/>
+      <c r="A27" s="11"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="11"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A28" s="2"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="2"/>
+      <c r="A28" s="11"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="11"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A29" s="2"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="2"/>
+      <c r="A29" s="11"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="11"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
     </row>
     <row r="30" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A30" s="2"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="2"/>
+      <c r="A30" s="11"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="11"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A31" s="2"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="2"/>
+      <c r="A31" s="11"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="11"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
     </row>
     <row r="32" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A32" s="2"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="2"/>
+      <c r="A32" s="11"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="11"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
     </row>
     <row r="33" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A33" s="2"/>
-      <c r="B33" s="10"/>
-      <c r="C33" s="2"/>
+      <c r="A33" s="11"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="11"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
     </row>
     <row r="34" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A34" s="2"/>
-      <c r="B34" s="10"/>
-      <c r="C34" s="2"/>
+      <c r="A34" s="11"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="11"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
     </row>
     <row r="35" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A35" s="2"/>
-      <c r="B35" s="10"/>
-      <c r="C35" s="2"/>
+      <c r="A35" s="11"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="11"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
     </row>
     <row r="36" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A36" s="2"/>
-      <c r="B36" s="10"/>
-      <c r="C36" s="2"/>
+      <c r="A36" s="11"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="11"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
     </row>
     <row r="37" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A37" s="2"/>
-      <c r="B37" s="10"/>
-      <c r="C37" s="2"/>
+      <c r="A37" s="11"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="11"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
     </row>
     <row r="38" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A38" s="2"/>
-      <c r="B38" s="10"/>
-      <c r="C38" s="2"/>
+      <c r="A38" s="11"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="11"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
     </row>
     <row r="39" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A39" s="2"/>
-      <c r="B39" s="10"/>
-      <c r="C39" s="2"/>
+      <c r="A39" s="11"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="11"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
     </row>
     <row r="40" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A40" s="2"/>
-      <c r="B40" s="10"/>
-      <c r="C40" s="2"/>
+      <c r="A40" s="11"/>
+      <c r="B40" s="15"/>
+      <c r="C40" s="11"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
     </row>
     <row r="41" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A41" s="2"/>
-      <c r="B41" s="10"/>
-      <c r="C41" s="2"/>
+      <c r="A41" s="11"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="11"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
     </row>
     <row r="42" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A42" s="2"/>
-      <c r="B42" s="10"/>
-      <c r="C42" s="2"/>
+      <c r="A42" s="11"/>
+      <c r="B42" s="15"/>
+      <c r="C42" s="11"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
     </row>
     <row r="43" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A43" s="2"/>
-      <c r="B43" s="10"/>
-      <c r="C43" s="2"/>
+      <c r="A43" s="11"/>
+      <c r="B43" s="15"/>
+      <c r="C43" s="11"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
     </row>
     <row r="44" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A44" s="2"/>
-      <c r="B44" s="10"/>
-      <c r="C44" s="2"/>
+      <c r="A44" s="11"/>
+      <c r="B44" s="15"/>
+      <c r="C44" s="11"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
     </row>
     <row r="45" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A45" s="2"/>
-      <c r="B45" s="10"/>
-      <c r="C45" s="2"/>
+      <c r="A45" s="11"/>
+      <c r="B45" s="15"/>
+      <c r="C45" s="11"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
     </row>
     <row r="46" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A46" s="2"/>
-      <c r="B46" s="10"/>
-      <c r="C46" s="2"/>
+      <c r="A46" s="11"/>
+      <c r="B46" s="15"/>
+      <c r="C46" s="11"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
     </row>
     <row r="47" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A47" s="2"/>
-      <c r="B47" s="10"/>
-      <c r="C47" s="2"/>
+      <c r="A47" s="11"/>
+      <c r="B47" s="15"/>
+      <c r="C47" s="11"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
     </row>
     <row r="48" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A48" s="2"/>
-      <c r="B48" s="10"/>
-      <c r="C48" s="2"/>
+      <c r="A48" s="11"/>
+      <c r="B48" s="15"/>
+      <c r="C48" s="11"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
     </row>
     <row r="49" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A49" s="2"/>
-      <c r="B49" s="10"/>
-      <c r="C49" s="2"/>
+      <c r="A49" s="11"/>
+      <c r="B49" s="15"/>
+      <c r="C49" s="11"/>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
     </row>
     <row r="50" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A50" s="2"/>
-      <c r="B50" s="10"/>
-      <c r="C50" s="2"/>
+      <c r="A50" s="11"/>
+      <c r="B50" s="15"/>
+      <c r="C50" s="11"/>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
     </row>
     <row r="51" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A51" s="2"/>
-      <c r="B51" s="10"/>
-      <c r="C51" s="2"/>
+      <c r="A51" s="11"/>
+      <c r="B51" s="15"/>
+      <c r="C51" s="11"/>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
     </row>
     <row r="52" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A52" s="2"/>
-      <c r="B52" s="10"/>
-      <c r="C52" s="2"/>
+      <c r="A52" s="11"/>
+      <c r="B52" s="15"/>
+      <c r="C52" s="11"/>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
     </row>
     <row r="53" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A53" s="2"/>
-      <c r="B53" s="10"/>
-      <c r="C53" s="2"/>
+      <c r="A53" s="11"/>
+      <c r="B53" s="15"/>
+      <c r="C53" s="11"/>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
     </row>
     <row r="54" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A54" s="2"/>
-      <c r="B54" s="10"/>
-      <c r="C54" s="2"/>
+      <c r="A54" s="11"/>
+      <c r="B54" s="15"/>
+      <c r="C54" s="11"/>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
     </row>
     <row r="55" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A55" s="2"/>
-      <c r="B55" s="10"/>
-      <c r="C55" s="2"/>
+      <c r="A55" s="11"/>
+      <c r="B55" s="15"/>
+      <c r="C55" s="11"/>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
     </row>
     <row r="56" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A56" s="2"/>
-      <c r="B56" s="10"/>
-      <c r="C56" s="2"/>
+      <c r="A56" s="11"/>
+      <c r="B56" s="15"/>
+      <c r="C56" s="11"/>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
       <c r="G56" s="2"/>
     </row>
     <row r="57" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A57" s="2"/>
-      <c r="B57" s="10"/>
-      <c r="C57" s="2"/>
+      <c r="A57" s="11"/>
+      <c r="B57" s="15"/>
+      <c r="C57" s="11"/>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
     </row>
     <row r="58" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A58" s="2"/>
-      <c r="B58" s="10"/>
-      <c r="C58" s="2"/>
+      <c r="A58" s="11"/>
+      <c r="B58" s="15"/>
+      <c r="C58" s="11"/>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
       <c r="G58" s="2"/>
     </row>
     <row r="59" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A59" s="2"/>
-      <c r="B59" s="10"/>
-      <c r="C59" s="2"/>
+      <c r="A59" s="11"/>
+      <c r="B59" s="15"/>
+      <c r="C59" s="11"/>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
       <c r="G59" s="2"/>
     </row>
     <row r="60" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A60" s="2"/>
-      <c r="B60" s="10"/>
-      <c r="C60" s="2"/>
+      <c r="A60" s="11"/>
+      <c r="B60" s="15"/>
+      <c r="C60" s="11"/>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
       <c r="G60" s="2"/>
     </row>
     <row r="61" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A61" s="2"/>
-      <c r="B61" s="10"/>
-      <c r="C61" s="2"/>
+      <c r="A61" s="11"/>
+      <c r="B61" s="15"/>
+      <c r="C61" s="11"/>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
     </row>
     <row r="62" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A62" s="2"/>
-      <c r="B62" s="10"/>
-      <c r="C62" s="2"/>
+      <c r="A62" s="11"/>
+      <c r="B62" s="15"/>
+      <c r="C62" s="11"/>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>
     </row>
     <row r="63" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A63" s="2"/>
-      <c r="B63" s="10"/>
-      <c r="C63" s="2"/>
+      <c r="A63" s="11"/>
+      <c r="B63" s="15"/>
+      <c r="C63" s="11"/>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
       <c r="G63" s="2"/>
     </row>
     <row r="64" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A64" s="2"/>
-      <c r="B64" s="10"/>
-      <c r="C64" s="2"/>
+      <c r="A64" s="11"/>
+      <c r="B64" s="15"/>
+      <c r="C64" s="11"/>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
     </row>
     <row r="65" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A65" s="2"/>
-      <c r="B65" s="10"/>
-      <c r="C65" s="2"/>
+      <c r="A65" s="11"/>
+      <c r="B65" s="15"/>
+      <c r="C65" s="11"/>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
       <c r="G65" s="2"/>
     </row>
     <row r="66" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A66" s="2"/>
-      <c r="B66" s="10"/>
-      <c r="C66" s="2"/>
+      <c r="A66" s="11"/>
+      <c r="B66" s="15"/>
+      <c r="C66" s="11"/>
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
     </row>
     <row r="67" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A67" s="2"/>
-      <c r="B67" s="10"/>
-      <c r="C67" s="2"/>
+      <c r="A67" s="11"/>
+      <c r="B67" s="15"/>
+      <c r="C67" s="11"/>
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
     </row>
     <row r="68" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A68" s="2"/>
-      <c r="B68" s="10"/>
-      <c r="C68" s="2"/>
+      <c r="A68" s="11"/>
+      <c r="B68" s="15"/>
+      <c r="C68" s="11"/>
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
       <c r="G68" s="2"/>
     </row>
     <row r="69" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A69" s="2"/>
-      <c r="B69" s="10"/>
-      <c r="C69" s="2"/>
+      <c r="A69" s="11"/>
+      <c r="B69" s="15"/>
+      <c r="C69" s="11"/>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
       <c r="G69" s="2"/>
     </row>
     <row r="70" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A70" s="2"/>
-      <c r="B70" s="10"/>
-      <c r="C70" s="2"/>
+      <c r="A70" s="11"/>
+      <c r="B70" s="15"/>
+      <c r="C70" s="11"/>
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
       <c r="G70" s="2"/>
     </row>
     <row r="71" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A71" s="2"/>
-      <c r="B71" s="10"/>
-      <c r="C71" s="2"/>
+      <c r="A71" s="11"/>
+      <c r="B71" s="15"/>
+      <c r="C71" s="11"/>
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
       <c r="G71" s="2"/>
     </row>
     <row r="72" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A72" s="2"/>
-      <c r="B72" s="10"/>
-      <c r="C72" s="2"/>
+      <c r="A72" s="11"/>
+      <c r="B72" s="15"/>
+      <c r="C72" s="11"/>
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
       <c r="G72" s="2"/>
     </row>
     <row r="73" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A73" s="2"/>
-      <c r="B73" s="10"/>
-      <c r="C73" s="2"/>
+      <c r="A73" s="11"/>
+      <c r="B73" s="15"/>
+      <c r="C73" s="11"/>
       <c r="D73" s="2"/>
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
       <c r="G73" s="2"/>
     </row>
     <row r="74" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A74" s="2"/>
-      <c r="B74" s="10"/>
-      <c r="C74" s="2"/>
+      <c r="A74" s="11"/>
+      <c r="B74" s="15"/>
+      <c r="C74" s="11"/>
       <c r="D74" s="2"/>
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
       <c r="G74" s="2"/>
     </row>
     <row r="75" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A75" s="2"/>
-      <c r="B75" s="10"/>
-      <c r="C75" s="2"/>
+      <c r="A75" s="11"/>
+      <c r="B75" s="15"/>
+      <c r="C75" s="11"/>
       <c r="D75" s="2"/>
       <c r="E75" s="2"/>
       <c r="F75" s="2"/>
       <c r="G75" s="2"/>
     </row>
     <row r="76" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A76" s="2"/>
-      <c r="B76" s="10"/>
-      <c r="C76" s="2"/>
+      <c r="A76" s="11"/>
+      <c r="B76" s="15"/>
+      <c r="C76" s="11"/>
       <c r="D76" s="2"/>
       <c r="E76" s="2"/>
       <c r="F76" s="2"/>
       <c r="G76" s="2"/>
     </row>
     <row r="77" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A77" s="2"/>
-      <c r="B77" s="10"/>
-      <c r="C77" s="2"/>
+      <c r="A77" s="11"/>
+      <c r="B77" s="15"/>
+      <c r="C77" s="11"/>
       <c r="D77" s="2"/>
       <c r="E77" s="2"/>
       <c r="F77" s="2"/>
       <c r="G77" s="2"/>
     </row>
     <row r="78" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A78" s="2"/>
-      <c r="B78" s="10"/>
-      <c r="C78" s="2"/>
+      <c r="A78" s="11"/>
+      <c r="B78" s="15"/>
+      <c r="C78" s="11"/>
       <c r="D78" s="2"/>
       <c r="E78" s="2"/>
       <c r="F78" s="2"/>
       <c r="G78" s="2"/>
     </row>
     <row r="79" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A79" s="2"/>
-      <c r="B79" s="10"/>
-      <c r="C79" s="2"/>
+      <c r="A79" s="11"/>
+      <c r="B79" s="15"/>
+      <c r="C79" s="11"/>
       <c r="D79" s="2"/>
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
       <c r="G79" s="2"/>
     </row>
     <row r="80" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A80" s="2"/>
-      <c r="B80" s="10"/>
-      <c r="C80" s="2"/>
+      <c r="A80" s="11"/>
+      <c r="B80" s="15"/>
+      <c r="C80" s="11"/>
       <c r="D80" s="2"/>
       <c r="E80" s="2"/>
       <c r="F80" s="2"/>
       <c r="G80" s="2"/>
     </row>
     <row r="81" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A81" s="2"/>
-      <c r="B81" s="10"/>
-      <c r="C81" s="2"/>
+      <c r="A81" s="11"/>
+      <c r="B81" s="15"/>
+      <c r="C81" s="11"/>
       <c r="D81" s="2"/>
       <c r="E81" s="2"/>
       <c r="F81" s="2"/>
       <c r="G81" s="2"/>
     </row>
     <row r="82" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A82" s="2"/>
-      <c r="B82" s="10"/>
-      <c r="C82" s="2"/>
+      <c r="A82" s="11"/>
+      <c r="B82" s="15"/>
+      <c r="C82" s="11"/>
       <c r="D82" s="2"/>
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
       <c r="G82" s="2"/>
     </row>
     <row r="83" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A83" s="2"/>
-      <c r="B83" s="10"/>
-      <c r="C83" s="2"/>
+      <c r="A83" s="11"/>
+      <c r="B83" s="15"/>
+      <c r="C83" s="11"/>
       <c r="D83" s="2"/>
       <c r="E83" s="2"/>
       <c r="F83" s="2"/>
       <c r="G83" s="2"/>
     </row>
     <row r="84" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A84" s="2"/>
-      <c r="B84" s="10"/>
-      <c r="C84" s="2"/>
+      <c r="A84" s="11"/>
+      <c r="B84" s="15"/>
+      <c r="C84" s="11"/>
       <c r="D84" s="2"/>
       <c r="E84" s="2"/>
       <c r="F84" s="2"/>
       <c r="G84" s="2"/>
     </row>
     <row r="85" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A85" s="2"/>
-      <c r="B85" s="10"/>
-      <c r="C85" s="2"/>
+      <c r="A85" s="11"/>
+      <c r="B85" s="15"/>
+      <c r="C85" s="11"/>
       <c r="D85" s="2"/>
       <c r="E85" s="2"/>
       <c r="F85" s="2"/>
       <c r="G85" s="2"/>
     </row>
     <row r="86" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A86" s="2"/>
-      <c r="B86" s="10"/>
-      <c r="C86" s="2"/>
+      <c r="A86" s="11"/>
+      <c r="B86" s="15"/>
+      <c r="C86" s="11"/>
       <c r="D86" s="2"/>
       <c r="E86" s="2"/>
       <c r="F86" s="2"/>
       <c r="G86" s="2"/>
     </row>
     <row r="87" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A87" s="2"/>
-      <c r="B87" s="10"/>
-      <c r="C87" s="2"/>
+      <c r="A87" s="11"/>
+      <c r="B87" s="15"/>
+      <c r="C87" s="11"/>
       <c r="D87" s="2"/>
       <c r="E87" s="2"/>
       <c r="F87" s="2"/>
       <c r="G87" s="2"/>
     </row>
     <row r="88" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A88" s="2"/>
-      <c r="B88" s="10"/>
-      <c r="C88" s="2"/>
+      <c r="A88" s="11"/>
+      <c r="B88" s="15"/>
+      <c r="C88" s="11"/>
       <c r="D88" s="2"/>
       <c r="E88" s="2"/>
       <c r="F88" s="2"/>
       <c r="G88" s="2"/>
     </row>
     <row r="89" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A89" s="2"/>
-      <c r="B89" s="10"/>
-      <c r="C89" s="2"/>
+      <c r="A89" s="11"/>
+      <c r="B89" s="15"/>
+      <c r="C89" s="11"/>
       <c r="D89" s="2"/>
       <c r="E89" s="2"/>
       <c r="F89" s="2"/>
       <c r="G89" s="2"/>
     </row>
     <row r="90" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A90" s="2"/>
-      <c r="B90" s="10"/>
-      <c r="C90" s="2"/>
+      <c r="A90" s="11"/>
+      <c r="B90" s="15"/>
+      <c r="C90" s="11"/>
       <c r="D90" s="2"/>
       <c r="E90" s="2"/>
       <c r="F90" s="2"/>
       <c r="G90" s="2"/>
     </row>
     <row r="91" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A91" s="2"/>
-      <c r="B91" s="10"/>
-      <c r="C91" s="2"/>
+      <c r="A91" s="11"/>
+      <c r="B91" s="15"/>
+      <c r="C91" s="11"/>
       <c r="D91" s="2"/>
       <c r="E91" s="2"/>
       <c r="F91" s="2"/>
       <c r="G91" s="2"/>
     </row>
     <row r="92" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A92" s="2"/>
-      <c r="B92" s="10"/>
-      <c r="C92" s="2"/>
+      <c r="A92" s="11"/>
+      <c r="B92" s="15"/>
+      <c r="C92" s="11"/>
       <c r="D92" s="2"/>
       <c r="E92" s="2"/>
       <c r="F92" s="2"/>
       <c r="G92" s="2"/>
     </row>
     <row r="93" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A93" s="2"/>
-      <c r="B93" s="10"/>
-      <c r="C93" s="2"/>
+      <c r="A93" s="11"/>
+      <c r="B93" s="15"/>
+      <c r="C93" s="11"/>
       <c r="D93" s="2"/>
       <c r="E93" s="2"/>
       <c r="F93" s="2"/>
       <c r="G93" s="2"/>
     </row>
     <row r="94" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A94" s="2"/>
-      <c r="B94" s="10"/>
-      <c r="C94" s="2"/>
+      <c r="A94" s="11"/>
+      <c r="B94" s="15"/>
+      <c r="C94" s="11"/>
       <c r="D94" s="2"/>
       <c r="E94" s="2"/>
       <c r="F94" s="2"/>
       <c r="G94" s="2"/>
     </row>
     <row r="95" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A95" s="2"/>
-      <c r="B95" s="10"/>
-      <c r="C95" s="2"/>
+      <c r="A95" s="11"/>
+      <c r="B95" s="15"/>
+      <c r="C95" s="11"/>
       <c r="D95" s="2"/>
       <c r="E95" s="2"/>
       <c r="F95" s="2"/>
       <c r="G95" s="2"/>
     </row>
     <row r="96" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A96" s="2"/>
-      <c r="B96" s="10"/>
-      <c r="C96" s="2"/>
+      <c r="A96" s="11"/>
+      <c r="B96" s="15"/>
+      <c r="C96" s="11"/>
       <c r="D96" s="2"/>
       <c r="E96" s="2"/>
       <c r="F96" s="2"/>
       <c r="G96" s="2"/>
     </row>
     <row r="97" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A97" s="2"/>
-      <c r="B97" s="10"/>
-      <c r="C97" s="2"/>
+      <c r="A97" s="11"/>
+      <c r="B97" s="15"/>
+      <c r="C97" s="11"/>
       <c r="D97" s="2"/>
       <c r="E97" s="2"/>
       <c r="F97" s="2"/>
       <c r="G97" s="2"/>
     </row>
     <row r="98" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A98" s="2"/>
-      <c r="B98" s="10"/>
-      <c r="C98" s="2"/>
+      <c r="A98" s="11"/>
+      <c r="B98" s="15"/>
+      <c r="C98" s="11"/>
       <c r="D98" s="2"/>
       <c r="E98" s="2"/>
       <c r="F98" s="2"/>
       <c r="G98" s="2"/>
     </row>
     <row r="99" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A99" s="2"/>
-      <c r="B99" s="10"/>
-      <c r="C99" s="2"/>
+      <c r="A99" s="11"/>
+      <c r="B99" s="15"/>
+      <c r="C99" s="11"/>
       <c r="D99" s="2"/>
       <c r="E99" s="2"/>
       <c r="F99" s="2"/>
       <c r="G99" s="2"/>
     </row>
     <row r="100" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A100" s="2"/>
-      <c r="B100" s="10"/>
-      <c r="C100" s="2"/>
+      <c r="A100" s="11"/>
+      <c r="B100" s="15"/>
+      <c r="C100" s="11"/>
       <c r="D100" s="2"/>
       <c r="E100" s="2"/>
       <c r="F100" s="2"/>
       <c r="G100" s="2"/>
     </row>
     <row r="101" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A101" s="2"/>
-      <c r="B101" s="10"/>
-      <c r="C101" s="2"/>
+      <c r="A101" s="11"/>
+      <c r="B101" s="15"/>
+      <c r="C101" s="11"/>
       <c r="D101" s="2"/>
       <c r="E101" s="2"/>
       <c r="F101" s="2"/>
       <c r="G101" s="2"/>
     </row>
     <row r="102" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A102" s="2"/>
-      <c r="B102" s="10"/>
-      <c r="C102" s="2"/>
+      <c r="A102" s="11"/>
+      <c r="B102" s="15"/>
+      <c r="C102" s="11"/>
       <c r="D102" s="2"/>
       <c r="E102" s="2"/>
       <c r="F102" s="2"/>
       <c r="G102" s="2"/>
     </row>
     <row r="103" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A103" s="2"/>
-      <c r="B103" s="10"/>
-      <c r="C103" s="2"/>
+      <c r="A103" s="11"/>
+      <c r="B103" s="15"/>
+      <c r="C103" s="11"/>
       <c r="D103" s="2"/>
       <c r="E103" s="2"/>
       <c r="F103" s="2"/>
       <c r="G103" s="2"/>
     </row>
     <row r="104" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A104" s="2"/>
-      <c r="B104" s="10"/>
-      <c r="C104" s="2"/>
+      <c r="A104" s="11"/>
+      <c r="B104" s="15"/>
+      <c r="C104" s="11"/>
       <c r="D104" s="2"/>
       <c r="E104" s="2"/>
       <c r="F104" s="2"/>
       <c r="G104" s="2"/>
     </row>
     <row r="105" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A105" s="2"/>
-      <c r="B105" s="10"/>
-      <c r="C105" s="2"/>
+      <c r="A105" s="11"/>
+      <c r="B105" s="15"/>
+      <c r="C105" s="11"/>
       <c r="D105" s="2"/>
       <c r="E105" s="2"/>
       <c r="F105" s="2"/>
       <c r="G105" s="2"/>
     </row>
     <row r="106" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A106" s="2"/>
-      <c r="B106" s="10"/>
-      <c r="C106" s="2"/>
+      <c r="A106" s="11"/>
+      <c r="B106" s="15"/>
+      <c r="C106" s="11"/>
       <c r="D106" s="2"/>
       <c r="E106" s="2"/>
       <c r="F106" s="2"/>
       <c r="G106" s="2"/>
     </row>
     <row r="107" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A107" s="2"/>
-      <c r="B107" s="10"/>
-      <c r="C107" s="2"/>
+      <c r="A107" s="11"/>
+      <c r="B107" s="15"/>
+      <c r="C107" s="11"/>
       <c r="D107" s="2"/>
       <c r="E107" s="2"/>
       <c r="F107" s="2"/>
       <c r="G107" s="2"/>
     </row>
     <row r="108" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A108" s="2"/>
-      <c r="B108" s="10"/>
-      <c r="C108" s="2"/>
+      <c r="A108" s="11"/>
+      <c r="B108" s="15"/>
+      <c r="C108" s="11"/>
       <c r="D108" s="2"/>
       <c r="E108" s="2"/>
       <c r="F108" s="2"/>
       <c r="G108" s="2"/>
     </row>
     <row r="109" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A109" s="2"/>
-      <c r="B109" s="10"/>
-      <c r="C109" s="2"/>
+      <c r="A109" s="11"/>
+      <c r="B109" s="15"/>
+      <c r="C109" s="11"/>
       <c r="D109" s="2"/>
       <c r="E109" s="2"/>
       <c r="F109" s="2"/>
       <c r="G109" s="2"/>
     </row>
     <row r="110" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A110" s="2"/>
-      <c r="B110" s="10"/>
-      <c r="C110" s="2"/>
+      <c r="A110" s="11"/>
+      <c r="B110" s="15"/>
+      <c r="C110" s="11"/>
       <c r="D110" s="2"/>
       <c r="E110" s="2"/>
       <c r="F110" s="2"/>
       <c r="G110" s="2"/>
     </row>
     <row r="111" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A111" s="2"/>
-      <c r="B111" s="10"/>
-      <c r="C111" s="2"/>
+      <c r="A111" s="11"/>
+      <c r="B111" s="15"/>
+      <c r="C111" s="11"/>
       <c r="D111" s="2"/>
       <c r="E111" s="2"/>
       <c r="F111" s="2"/>
       <c r="G111" s="2"/>
     </row>
     <row r="112" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A112" s="2"/>
-      <c r="B112" s="10"/>
-      <c r="C112" s="2"/>
+      <c r="A112" s="11"/>
+      <c r="B112" s="15"/>
+      <c r="C112" s="11"/>
       <c r="D112" s="2"/>
       <c r="E112" s="2"/>
       <c r="F112" s="2"/>
       <c r="G112" s="2"/>
     </row>
     <row r="113" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A113" s="2"/>
-      <c r="B113" s="10"/>
-      <c r="C113" s="2"/>
+      <c r="A113" s="11"/>
+      <c r="B113" s="15"/>
+      <c r="C113" s="11"/>
       <c r="D113" s="2"/>
       <c r="E113" s="2"/>
       <c r="F113" s="2"/>
       <c r="G113" s="2"/>
     </row>
     <row r="114" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A114" s="2"/>
-      <c r="B114" s="10"/>
-      <c r="C114" s="2"/>
+      <c r="A114" s="11"/>
+      <c r="B114" s="15"/>
+      <c r="C114" s="11"/>
       <c r="D114" s="2"/>
       <c r="E114" s="2"/>
       <c r="F114" s="2"/>
       <c r="G114" s="2"/>
     </row>
     <row r="115" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A115" s="2"/>
-      <c r="B115" s="10"/>
-      <c r="C115" s="2"/>
+      <c r="A115" s="11"/>
+      <c r="B115" s="15"/>
+      <c r="C115" s="11"/>
       <c r="D115" s="2"/>
       <c r="E115" s="2"/>
       <c r="F115" s="2"/>
       <c r="G115" s="2"/>
     </row>
     <row r="116" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A116" s="2"/>
-      <c r="B116" s="10"/>
-      <c r="C116" s="2"/>
+      <c r="A116" s="11"/>
+      <c r="B116" s="15"/>
+      <c r="C116" s="11"/>
       <c r="D116" s="2"/>
       <c r="E116" s="2"/>
       <c r="F116" s="2"/>
       <c r="G116" s="2"/>
     </row>
     <row r="117" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A117" s="2"/>
-      <c r="B117" s="10"/>
-      <c r="C117" s="2"/>
+      <c r="A117" s="11"/>
+      <c r="B117" s="15"/>
+      <c r="C117" s="11"/>
       <c r="D117" s="2"/>
       <c r="E117" s="2"/>
       <c r="F117" s="2"/>
       <c r="G117" s="2"/>
     </row>
     <row r="118" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A118" s="2"/>
-      <c r="B118" s="10"/>
-      <c r="C118" s="2"/>
+      <c r="A118" s="11"/>
+      <c r="B118" s="15"/>
+      <c r="C118" s="11"/>
       <c r="D118" s="2"/>
       <c r="E118" s="2"/>
       <c r="F118" s="2"/>
       <c r="G118" s="2"/>
     </row>
     <row r="119" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A119" s="2"/>
-      <c r="B119" s="10"/>
-      <c r="C119" s="2"/>
+      <c r="A119" s="11"/>
+      <c r="B119" s="15"/>
+      <c r="C119" s="11"/>
       <c r="D119" s="2"/>
       <c r="E119" s="2"/>
       <c r="F119" s="2"/>
       <c r="G119" s="2"/>
     </row>
     <row r="120" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A120" s="2"/>
-      <c r="B120" s="10"/>
-      <c r="C120" s="2"/>
+      <c r="A120" s="11"/>
+      <c r="B120" s="15"/>
+      <c r="C120" s="11"/>
       <c r="D120" s="2"/>
       <c r="E120" s="2"/>
       <c r="F120" s="2"/>
       <c r="G120" s="2"/>
     </row>
     <row r="121" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A121" s="2"/>
-      <c r="B121" s="10"/>
-      <c r="C121" s="2"/>
+      <c r="A121" s="11"/>
+      <c r="B121" s="15"/>
+      <c r="C121" s="11"/>
       <c r="D121" s="2"/>
       <c r="E121" s="2"/>
       <c r="F121" s="2"/>
       <c r="G121" s="2"/>
     </row>
     <row r="122" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A122" s="2"/>
-      <c r="B122" s="10"/>
-      <c r="C122" s="2"/>
+      <c r="A122" s="11"/>
+      <c r="B122" s="15"/>
+      <c r="C122" s="11"/>
       <c r="D122" s="2"/>
       <c r="E122" s="2"/>
       <c r="F122" s="2"/>
       <c r="G122" s="2"/>
     </row>
     <row r="123" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A123" s="2"/>
-      <c r="B123" s="10"/>
-      <c r="C123" s="2"/>
+      <c r="A123" s="11"/>
+      <c r="B123" s="15"/>
+      <c r="C123" s="11"/>
       <c r="D123" s="2"/>
       <c r="E123" s="2"/>
       <c r="F123" s="2"/>
       <c r="G123" s="2"/>
     </row>
     <row r="124" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A124" s="2"/>
-      <c r="B124" s="10"/>
-      <c r="C124" s="2"/>
+      <c r="A124" s="11"/>
+      <c r="B124" s="15"/>
+      <c r="C124" s="11"/>
       <c r="D124" s="2"/>
       <c r="E124" s="2"/>
       <c r="F124" s="2"/>
       <c r="G124" s="2"/>
     </row>
     <row r="125" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A125" s="2"/>
-      <c r="B125" s="10"/>
-      <c r="C125" s="2"/>
+      <c r="A125" s="11"/>
+      <c r="B125" s="15"/>
+      <c r="C125" s="11"/>
       <c r="D125" s="2"/>
       <c r="E125" s="2"/>
       <c r="F125" s="2"/>
       <c r="G125" s="2"/>
     </row>
     <row r="126" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A126" s="2"/>
-      <c r="B126" s="10"/>
-      <c r="C126" s="2"/>
+      <c r="A126" s="11"/>
+      <c r="B126" s="15"/>
+      <c r="C126" s="11"/>
       <c r="D126" s="2"/>
       <c r="E126" s="2"/>
       <c r="F126" s="2"/>
       <c r="G126" s="2"/>
     </row>
     <row r="127" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A127" s="2"/>
-      <c r="B127" s="10"/>
-      <c r="C127" s="2"/>
+      <c r="A127" s="11"/>
+      <c r="B127" s="15"/>
+      <c r="C127" s="11"/>
       <c r="D127" s="2"/>
       <c r="E127" s="2"/>
       <c r="F127" s="2"/>
       <c r="G127" s="2"/>
     </row>
     <row r="128" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A128" s="2"/>
-      <c r="B128" s="10"/>
-      <c r="C128" s="2"/>
+      <c r="A128" s="11"/>
+      <c r="B128" s="15"/>
+      <c r="C128" s="11"/>
       <c r="D128" s="2"/>
       <c r="E128" s="2"/>
       <c r="F128" s="2"/>
       <c r="G128" s="2"/>
     </row>
     <row r="129" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A129" s="2"/>
-      <c r="B129" s="10"/>
-      <c r="C129" s="2"/>
+      <c r="A129" s="11"/>
+      <c r="B129" s="15"/>
+      <c r="C129" s="11"/>
       <c r="D129" s="2"/>
       <c r="E129" s="2"/>
       <c r="F129" s="2"/>
       <c r="G129" s="2"/>
     </row>
     <row r="130" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A130" s="2"/>
-      <c r="B130" s="10"/>
-      <c r="C130" s="2"/>
+      <c r="A130" s="11"/>
+      <c r="B130" s="15"/>
+      <c r="C130" s="11"/>
       <c r="D130" s="2"/>
       <c r="E130" s="2"/>
       <c r="F130" s="2"/>
       <c r="G130" s="2"/>
     </row>
     <row r="131" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A131" s="2"/>
-      <c r="B131" s="10"/>
-      <c r="C131" s="2"/>
+      <c r="A131" s="11"/>
+      <c r="B131" s="15"/>
+      <c r="C131" s="11"/>
       <c r="D131" s="2"/>
       <c r="E131" s="2"/>
       <c r="F131" s="2"/>
       <c r="G131" s="2"/>
     </row>
     <row r="132" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A132" s="2"/>
-      <c r="B132" s="10"/>
-      <c r="C132" s="2"/>
+      <c r="A132" s="11"/>
+      <c r="B132" s="15"/>
+      <c r="C132" s="11"/>
       <c r="D132" s="2"/>
       <c r="E132" s="2"/>
       <c r="F132" s="2"/>
       <c r="G132" s="2"/>
     </row>
     <row r="133" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A133" s="2"/>
-      <c r="B133" s="10"/>
-      <c r="C133" s="2"/>
+      <c r="A133" s="11"/>
+      <c r="B133" s="15"/>
+      <c r="C133" s="11"/>
       <c r="D133" s="2"/>
       <c r="E133" s="2"/>
       <c r="F133" s="2"/>
       <c r="G133" s="2"/>
     </row>
     <row r="134" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A134" s="2"/>
-      <c r="B134" s="10"/>
-      <c r="C134" s="2"/>
+      <c r="A134" s="11"/>
+      <c r="B134" s="15"/>
+      <c r="C134" s="11"/>
       <c r="D134" s="2"/>
       <c r="E134" s="2"/>
       <c r="F134" s="2"/>
       <c r="G134" s="2"/>
     </row>
     <row r="135" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A135" s="2"/>
-      <c r="B135" s="10"/>
-      <c r="C135" s="2"/>
+      <c r="A135" s="11"/>
+      <c r="B135" s="15"/>
+      <c r="C135" s="11"/>
       <c r="D135" s="2"/>
       <c r="E135" s="2"/>
       <c r="F135" s="2"/>
       <c r="G135" s="2"/>
     </row>
     <row r="136" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A136" s="2"/>
-      <c r="B136" s="10"/>
-      <c r="C136" s="2"/>
+      <c r="A136" s="11"/>
+      <c r="B136" s="15"/>
+      <c r="C136" s="11"/>
       <c r="D136" s="2"/>
       <c r="E136" s="2"/>
       <c r="F136" s="2"/>
       <c r="G136" s="2"/>
     </row>
     <row r="137" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A137" s="2"/>
-      <c r="B137" s="10"/>
-      <c r="C137" s="2"/>
+      <c r="A137" s="11"/>
+      <c r="B137" s="15"/>
+      <c r="C137" s="11"/>
       <c r="D137" s="2"/>
       <c r="E137" s="2"/>
       <c r="F137" s="2"/>
       <c r="G137" s="2"/>
     </row>
     <row r="138" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A138" s="2"/>
-      <c r="B138" s="10"/>
-      <c r="C138" s="2"/>
+      <c r="A138" s="11"/>
+      <c r="B138" s="15"/>
+      <c r="C138" s="11"/>
       <c r="D138" s="2"/>
       <c r="E138" s="2"/>
       <c r="F138" s="2"/>
       <c r="G138" s="2"/>
     </row>
     <row r="139" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A139" s="2"/>
-      <c r="B139" s="10"/>
-      <c r="C139" s="2"/>
+      <c r="A139" s="11"/>
+      <c r="B139" s="15"/>
+      <c r="C139" s="11"/>
       <c r="D139" s="2"/>
       <c r="E139" s="2"/>
       <c r="F139" s="2"/>
       <c r="G139" s="2"/>
     </row>
     <row r="140" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A140" s="2"/>
-      <c r="B140" s="10"/>
-      <c r="C140" s="2"/>
+      <c r="A140" s="11"/>
+      <c r="B140" s="15"/>
+      <c r="C140" s="11"/>
       <c r="D140" s="2"/>
       <c r="E140" s="2"/>
       <c r="F140" s="2"/>
       <c r="G140" s="2"/>
     </row>
     <row r="141" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A141" s="2"/>
-      <c r="B141" s="10"/>
-      <c r="C141" s="2"/>
+      <c r="A141" s="11"/>
+      <c r="B141" s="15"/>
+      <c r="C141" s="11"/>
       <c r="D141" s="2"/>
       <c r="E141" s="2"/>
       <c r="F141" s="2"/>
       <c r="G141" s="2"/>
     </row>
     <row r="142" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A142" s="2"/>
-      <c r="B142" s="10"/>
-      <c r="C142" s="2"/>
+      <c r="A142" s="11"/>
+      <c r="B142" s="15"/>
+      <c r="C142" s="11"/>
       <c r="D142" s="2"/>
       <c r="E142" s="2"/>
       <c r="F142" s="2"/>
       <c r="G142" s="2"/>
     </row>
     <row r="143" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A143" s="2"/>
-      <c r="B143" s="10"/>
-      <c r="C143" s="2"/>
+      <c r="A143" s="11"/>
+      <c r="B143" s="15"/>
+      <c r="C143" s="11"/>
       <c r="D143" s="2"/>
       <c r="E143" s="2"/>
       <c r="F143" s="2"/>
       <c r="G143" s="2"/>
     </row>
     <row r="144" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A144" s="2"/>
-      <c r="B144" s="10"/>
-      <c r="C144" s="2"/>
+      <c r="A144" s="11"/>
+      <c r="B144" s="15"/>
+      <c r="C144" s="11"/>
       <c r="D144" s="2"/>
       <c r="E144" s="2"/>
       <c r="F144" s="2"/>
       <c r="G144" s="2"/>
     </row>
     <row r="145" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A145" s="2"/>
-      <c r="B145" s="10"/>
-      <c r="C145" s="2"/>
+      <c r="A145" s="11"/>
+      <c r="B145" s="15"/>
+      <c r="C145" s="11"/>
       <c r="D145" s="2"/>
       <c r="E145" s="2"/>
       <c r="F145" s="2"/>
       <c r="G145" s="2"/>
     </row>
     <row r="146" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A146" s="2"/>
-      <c r="B146" s="10"/>
-      <c r="C146" s="2"/>
+      <c r="A146" s="11"/>
+      <c r="B146" s="15"/>
+      <c r="C146" s="11"/>
       <c r="D146" s="2"/>
       <c r="E146" s="2"/>
       <c r="F146" s="2"/>
       <c r="G146" s="2"/>
     </row>
     <row r="147" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A147" s="2"/>
-      <c r="B147" s="10"/>
-      <c r="C147" s="2"/>
+      <c r="A147" s="11"/>
+      <c r="B147" s="15"/>
+      <c r="C147" s="11"/>
       <c r="D147" s="2"/>
       <c r="E147" s="2"/>
       <c r="F147" s="2"/>
       <c r="G147" s="2"/>
     </row>
     <row r="148" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A148" s="2"/>
-      <c r="B148" s="10"/>
-      <c r="C148" s="2"/>
+      <c r="A148" s="11"/>
+      <c r="B148" s="15"/>
+      <c r="C148" s="11"/>
       <c r="D148" s="2"/>
       <c r="E148" s="2"/>
       <c r="F148" s="2"/>
       <c r="G148" s="2"/>
     </row>
     <row r="149" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A149" s="2"/>
-      <c r="B149" s="10"/>
-      <c r="C149" s="2"/>
+      <c r="A149" s="11"/>
+      <c r="B149" s="15"/>
+      <c r="C149" s="11"/>
       <c r="D149" s="2"/>
       <c r="E149" s="2"/>
       <c r="F149" s="2"/>
       <c r="G149" s="2"/>
     </row>
     <row r="150" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A150" s="2"/>
-      <c r="B150" s="10"/>
-      <c r="C150" s="2"/>
+      <c r="A150" s="11"/>
+      <c r="B150" s="15"/>
+      <c r="C150" s="11"/>
       <c r="D150" s="2"/>
       <c r="E150" s="2"/>
       <c r="F150" s="2"/>
       <c r="G150" s="2"/>
     </row>
     <row r="151" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A151" s="2"/>
-      <c r="B151" s="10"/>
-      <c r="C151" s="2"/>
+      <c r="A151" s="11"/>
+      <c r="B151" s="15"/>
+      <c r="C151" s="11"/>
       <c r="D151" s="2"/>
       <c r="E151" s="2"/>
       <c r="F151" s="2"/>
       <c r="G151" s="2"/>
     </row>
     <row r="152" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A152" s="2"/>
-      <c r="B152" s="10"/>
-      <c r="C152" s="2"/>
+      <c r="A152" s="11"/>
+      <c r="B152" s="15"/>
+      <c r="C152" s="11"/>
       <c r="D152" s="2"/>
       <c r="E152" s="2"/>
       <c r="F152" s="2"/>
       <c r="G152" s="2"/>
     </row>
     <row r="153" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A153" s="2"/>
-      <c r="B153" s="10"/>
-      <c r="C153" s="2"/>
+      <c r="A153" s="11"/>
+      <c r="B153" s="15"/>
+      <c r="C153" s="11"/>
       <c r="D153" s="2"/>
       <c r="E153" s="2"/>
       <c r="F153" s="2"/>
       <c r="G153" s="2"/>
     </row>
     <row r="154" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A154" s="2"/>
-      <c r="B154" s="10"/>
-      <c r="C154" s="2"/>
+      <c r="A154" s="11"/>
+      <c r="B154" s="15"/>
+      <c r="C154" s="11"/>
       <c r="D154" s="2"/>
       <c r="E154" s="2"/>
       <c r="F154" s="2"/>
       <c r="G154" s="2"/>
     </row>
     <row r="155" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A155" s="2"/>
-      <c r="B155" s="10"/>
-      <c r="C155" s="2"/>
+      <c r="A155" s="11"/>
+      <c r="B155" s="15"/>
+      <c r="C155" s="11"/>
       <c r="D155" s="2"/>
       <c r="E155" s="2"/>
       <c r="F155" s="2"/>
       <c r="G155" s="2"/>
     </row>
     <row r="156" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A156" s="2"/>
-      <c r="B156" s="10"/>
-      <c r="C156" s="2"/>
+      <c r="A156" s="11"/>
+      <c r="B156" s="15"/>
+      <c r="C156" s="11"/>
       <c r="D156" s="2"/>
       <c r="E156" s="2"/>
       <c r="F156" s="2"/>
       <c r="G156" s="2"/>
     </row>
     <row r="157" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A157" s="2"/>
-      <c r="B157" s="10"/>
-      <c r="C157" s="2"/>
+      <c r="A157" s="11"/>
+      <c r="B157" s="15"/>
+      <c r="C157" s="11"/>
       <c r="D157" s="2"/>
       <c r="E157" s="2"/>
       <c r="F157" s="2"/>
       <c r="G157" s="2"/>
     </row>
     <row r="158" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A158" s="2"/>
-      <c r="B158" s="10"/>
-      <c r="C158" s="2"/>
+      <c r="A158" s="11"/>
+      <c r="B158" s="15"/>
+      <c r="C158" s="11"/>
       <c r="D158" s="2"/>
       <c r="E158" s="2"/>
       <c r="F158" s="2"/>
       <c r="G158" s="2"/>
     </row>
     <row r="159" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A159" s="2"/>
-      <c r="B159" s="10"/>
-      <c r="C159" s="2"/>
+      <c r="A159" s="11"/>
+      <c r="B159" s="15"/>
+      <c r="C159" s="11"/>
       <c r="D159" s="2"/>
       <c r="E159" s="2"/>
       <c r="F159" s="2"/>
       <c r="G159" s="2"/>
     </row>
     <row r="160" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A160" s="2"/>
-      <c r="B160" s="10"/>
-      <c r="C160" s="2"/>
+      <c r="A160" s="11"/>
+      <c r="B160" s="15"/>
+      <c r="C160" s="11"/>
       <c r="D160" s="2"/>
       <c r="E160" s="2"/>
       <c r="F160" s="2"/>
       <c r="G160" s="2"/>
     </row>
     <row r="161" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A161" s="2"/>
-      <c r="B161" s="10"/>
-      <c r="C161" s="2"/>
+      <c r="A161" s="11"/>
+      <c r="B161" s="15"/>
+      <c r="C161" s="11"/>
       <c r="D161" s="2"/>
       <c r="E161" s="2"/>
       <c r="F161" s="2"/>
       <c r="G161" s="2"/>
     </row>
     <row r="162" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A162" s="2"/>
-      <c r="B162" s="10"/>
-      <c r="C162" s="2"/>
+      <c r="A162" s="11"/>
+      <c r="B162" s="15"/>
+      <c r="C162" s="11"/>
       <c r="D162" s="2"/>
       <c r="E162" s="2"/>
       <c r="F162" s="2"/>
       <c r="G162" s="2"/>
     </row>
     <row r="163" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A163" s="2"/>
-      <c r="B163" s="10"/>
-      <c r="C163" s="2"/>
+      <c r="A163" s="11"/>
+      <c r="B163" s="15"/>
+      <c r="C163" s="11"/>
       <c r="D163" s="2"/>
       <c r="E163" s="2"/>
       <c r="F163" s="2"/>
       <c r="G163" s="2"/>
     </row>
     <row r="164" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A164" s="2"/>
-      <c r="B164" s="10"/>
-      <c r="C164" s="2"/>
+      <c r="A164" s="11"/>
+      <c r="B164" s="15"/>
+      <c r="C164" s="11"/>
       <c r="D164" s="2"/>
       <c r="E164" s="2"/>
       <c r="F164" s="2"/>
       <c r="G164" s="2"/>
     </row>
     <row r="165" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A165" s="2"/>
-      <c r="B165" s="10"/>
-      <c r="C165" s="2"/>
+      <c r="A165" s="11"/>
+      <c r="B165" s="15"/>
+      <c r="C165" s="11"/>
       <c r="D165" s="2"/>
       <c r="E165" s="2"/>
       <c r="F165" s="2"/>
       <c r="G165" s="2"/>
     </row>
     <row r="166" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A166" s="2"/>
-      <c r="B166" s="10"/>
-      <c r="C166" s="2"/>
+      <c r="A166" s="11"/>
+      <c r="B166" s="15"/>
+      <c r="C166" s="11"/>
       <c r="D166" s="2"/>
       <c r="E166" s="2"/>
       <c r="F166" s="2"/>
       <c r="G166" s="2"/>
     </row>
     <row r="167" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A167" s="2"/>
-      <c r="B167" s="10"/>
-      <c r="C167" s="2"/>
+      <c r="A167" s="11"/>
+      <c r="B167" s="15"/>
+      <c r="C167" s="11"/>
       <c r="D167" s="2"/>
       <c r="E167" s="2"/>
       <c r="F167" s="2"/>
       <c r="G167" s="2"/>
     </row>
     <row r="168" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A168" s="2"/>
-      <c r="B168" s="10"/>
-      <c r="C168" s="2"/>
+      <c r="A168" s="11"/>
+      <c r="B168" s="15"/>
+      <c r="C168" s="11"/>
       <c r="D168" s="2"/>
       <c r="E168" s="2"/>
       <c r="F168" s="2"/>
       <c r="G168" s="2"/>
     </row>
     <row r="169" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A169" s="2"/>
-      <c r="B169" s="10"/>
-      <c r="C169" s="2"/>
+      <c r="A169" s="11"/>
+      <c r="B169" s="15"/>
+      <c r="C169" s="11"/>
       <c r="D169" s="2"/>
       <c r="E169" s="2"/>
       <c r="F169" s="2"/>
       <c r="G169" s="2"/>
     </row>
     <row r="170" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A170" s="2"/>
-      <c r="B170" s="10"/>
-      <c r="C170" s="2"/>
+      <c r="A170" s="11"/>
+      <c r="B170" s="15"/>
+      <c r="C170" s="11"/>
       <c r="D170" s="2"/>
       <c r="E170" s="2"/>
       <c r="F170" s="2"/>
       <c r="G170" s="2"/>
     </row>
     <row r="171" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A171" s="2"/>
-      <c r="B171" s="10"/>
-      <c r="C171" s="2"/>
+      <c r="A171" s="11"/>
+      <c r="B171" s="15"/>
+      <c r="C171" s="11"/>
       <c r="D171" s="2"/>
       <c r="E171" s="2"/>
       <c r="F171" s="2"/>
       <c r="G171" s="2"/>
     </row>
     <row r="172" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A172" s="2"/>
-      <c r="B172" s="10"/>
-      <c r="C172" s="2"/>
+      <c r="A172" s="11"/>
+      <c r="B172" s="15"/>
+      <c r="C172" s="11"/>
       <c r="D172" s="2"/>
       <c r="E172" s="2"/>
       <c r="F172" s="2"/>
       <c r="G172" s="2"/>
     </row>
     <row r="173" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A173" s="2"/>
-      <c r="B173" s="10"/>
-      <c r="C173" s="2"/>
+      <c r="A173" s="11"/>
+      <c r="B173" s="15"/>
+      <c r="C173" s="11"/>
       <c r="D173" s="2"/>
       <c r="E173" s="2"/>
       <c r="F173" s="2"/>
       <c r="G173" s="2"/>
     </row>
     <row r="174" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A174" s="2"/>
-      <c r="B174" s="10"/>
-      <c r="C174" s="2"/>
+      <c r="A174" s="11"/>
+      <c r="B174" s="15"/>
+      <c r="C174" s="11"/>
       <c r="D174" s="2"/>
       <c r="E174" s="2"/>
       <c r="F174" s="2"/>
       <c r="G174" s="2"/>
     </row>
     <row r="175" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A175" s="2"/>
-      <c r="B175" s="10"/>
-      <c r="C175" s="2"/>
+      <c r="A175" s="11"/>
+      <c r="B175" s="15"/>
+      <c r="C175" s="11"/>
       <c r="D175" s="2"/>
       <c r="E175" s="2"/>
       <c r="F175" s="2"/>
       <c r="G175" s="2"/>
     </row>
     <row r="176" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A176" s="2"/>
-      <c r="B176" s="10"/>
-      <c r="C176" s="2"/>
+      <c r="A176" s="11"/>
+      <c r="B176" s="15"/>
+      <c r="C176" s="11"/>
       <c r="D176" s="2"/>
       <c r="E176" s="2"/>
       <c r="F176" s="2"/>
       <c r="G176" s="2"/>
     </row>
     <row r="177" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A177" s="2"/>
-      <c r="B177" s="10"/>
-      <c r="C177" s="2"/>
+      <c r="A177" s="11"/>
+      <c r="B177" s="15"/>
+      <c r="C177" s="11"/>
       <c r="D177" s="2"/>
       <c r="E177" s="2"/>
       <c r="F177" s="2"/>
       <c r="G177" s="2"/>
     </row>
     <row r="178" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A178" s="2"/>
-      <c r="B178" s="10"/>
-      <c r="C178" s="2"/>
+      <c r="A178" s="11"/>
+      <c r="B178" s="15"/>
+      <c r="C178" s="11"/>
       <c r="D178" s="2"/>
       <c r="E178" s="2"/>
       <c r="F178" s="2"/>
       <c r="G178" s="2"/>
     </row>
     <row r="179" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A179" s="2"/>
-      <c r="B179" s="10"/>
-      <c r="C179" s="2"/>
+      <c r="A179" s="11"/>
+      <c r="B179" s="15"/>
+      <c r="C179" s="11"/>
       <c r="D179" s="2"/>
       <c r="E179" s="2"/>
       <c r="F179" s="2"/>
       <c r="G179" s="2"/>
     </row>
     <row r="180" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A180" s="2"/>
-      <c r="B180" s="10"/>
-      <c r="C180" s="2"/>
+      <c r="A180" s="11"/>
+      <c r="B180" s="15"/>
+      <c r="C180" s="11"/>
       <c r="D180" s="2"/>
       <c r="E180" s="2"/>
       <c r="F180" s="2"/>
       <c r="G180" s="2"/>
     </row>
     <row r="181" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A181" s="2"/>
-      <c r="B181" s="10"/>
-      <c r="C181" s="2"/>
+      <c r="A181" s="11"/>
+      <c r="B181" s="15"/>
+      <c r="C181" s="11"/>
       <c r="D181" s="2"/>
       <c r="E181" s="2"/>
       <c r="F181" s="2"/>
       <c r="G181" s="2"/>
     </row>
     <row r="182" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A182" s="2"/>
-      <c r="B182" s="10"/>
-      <c r="C182" s="2"/>
+      <c r="A182" s="11"/>
+      <c r="B182" s="15"/>
+      <c r="C182" s="11"/>
       <c r="D182" s="2"/>
       <c r="E182" s="2"/>
       <c r="F182" s="2"/>
       <c r="G182" s="2"/>
     </row>
     <row r="183" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A183" s="2"/>
-      <c r="B183" s="10"/>
-      <c r="C183" s="2"/>
+      <c r="A183" s="11"/>
+      <c r="B183" s="15"/>
+      <c r="C183" s="11"/>
       <c r="D183" s="2"/>
       <c r="E183" s="2"/>
       <c r="F183" s="2"/>
       <c r="G183" s="2"/>
     </row>
     <row r="184" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A184" s="2"/>
-      <c r="B184" s="10"/>
-      <c r="C184" s="2"/>
+      <c r="A184" s="11"/>
+      <c r="B184" s="15"/>
+      <c r="C184" s="11"/>
       <c r="D184" s="2"/>
       <c r="E184" s="2"/>
       <c r="F184" s="2"/>
       <c r="G184" s="2"/>
     </row>
     <row r="185" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A185" s="2"/>
-      <c r="B185" s="10"/>
-      <c r="C185" s="2"/>
+      <c r="A185" s="11"/>
+      <c r="B185" s="15"/>
+      <c r="C185" s="11"/>
       <c r="D185" s="2"/>
       <c r="E185" s="2"/>
       <c r="F185" s="2"/>
       <c r="G185" s="2"/>
     </row>
     <row r="186" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A186" s="2"/>
-      <c r="B186" s="10"/>
-      <c r="C186" s="2"/>
+      <c r="A186" s="11"/>
+      <c r="B186" s="15"/>
+      <c r="C186" s="11"/>
       <c r="D186" s="2"/>
       <c r="E186" s="2"/>
       <c r="F186" s="2"/>
       <c r="G186" s="2"/>
     </row>
     <row r="187" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A187" s="2"/>
-      <c r="B187" s="10"/>
-      <c r="C187" s="2"/>
+      <c r="A187" s="11"/>
+      <c r="B187" s="15"/>
+      <c r="C187" s="11"/>
       <c r="D187" s="2"/>
       <c r="E187" s="2"/>
       <c r="F187" s="2"/>
       <c r="G187" s="2"/>
     </row>
     <row r="188" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A188" s="2"/>
-      <c r="B188" s="10"/>
-      <c r="C188" s="2"/>
+      <c r="A188" s="11"/>
+      <c r="B188" s="15"/>
+      <c r="C188" s="11"/>
       <c r="D188" s="2"/>
       <c r="E188" s="2"/>
       <c r="F188" s="2"/>
       <c r="G188" s="2"/>
     </row>
     <row r="189" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A189" s="2"/>
-      <c r="B189" s="10"/>
-      <c r="C189" s="2"/>
+      <c r="A189" s="11"/>
+      <c r="B189" s="15"/>
+      <c r="C189" s="11"/>
       <c r="D189" s="2"/>
       <c r="E189" s="2"/>
       <c r="F189" s="2"/>
       <c r="G189" s="2"/>
     </row>
     <row r="190" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A190" s="2"/>
-      <c r="B190" s="10"/>
-      <c r="C190" s="2"/>
+      <c r="A190" s="11"/>
+      <c r="B190" s="15"/>
+      <c r="C190" s="11"/>
       <c r="D190" s="2"/>
       <c r="E190" s="2"/>
       <c r="F190" s="2"/>
       <c r="G190" s="2"/>
     </row>
     <row r="191" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A191" s="2"/>
-      <c r="B191" s="10"/>
-      <c r="C191" s="2"/>
+      <c r="A191" s="11"/>
+      <c r="B191" s="15"/>
+      <c r="C191" s="11"/>
       <c r="D191" s="2"/>
       <c r="E191" s="2"/>
       <c r="F191" s="2"/>
       <c r="G191" s="2"/>
     </row>
     <row r="192" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A192" s="2"/>
-      <c r="B192" s="10"/>
-      <c r="C192" s="2"/>
+      <c r="A192" s="11"/>
+      <c r="B192" s="15"/>
+      <c r="C192" s="11"/>
       <c r="D192" s="2"/>
       <c r="E192" s="2"/>
       <c r="F192" s="2"/>
       <c r="G192" s="2"/>
     </row>
     <row r="193" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A193" s="2"/>
-      <c r="B193" s="10"/>
-      <c r="C193" s="2"/>
+      <c r="A193" s="11"/>
+      <c r="B193" s="15"/>
+      <c r="C193" s="11"/>
       <c r="D193" s="2"/>
       <c r="E193" s="2"/>
       <c r="F193" s="2"/>
       <c r="G193" s="2"/>
     </row>
     <row r="194" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A194" s="2"/>
-      <c r="B194" s="10"/>
-      <c r="C194" s="2"/>
+      <c r="A194" s="11"/>
+      <c r="B194" s="15"/>
+      <c r="C194" s="11"/>
       <c r="D194" s="2"/>
       <c r="E194" s="2"/>
       <c r="F194" s="2"/>
       <c r="G194" s="2"/>
     </row>
     <row r="195" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A195" s="2"/>
-      <c r="B195" s="10"/>
-      <c r="C195" s="2"/>
+      <c r="A195" s="11"/>
+      <c r="B195" s="15"/>
+      <c r="C195" s="11"/>
       <c r="D195" s="2"/>
       <c r="E195" s="2"/>
       <c r="F195" s="2"/>
       <c r="G195" s="2"/>
     </row>
     <row r="196" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A196" s="2"/>
-      <c r="B196" s="10"/>
-      <c r="C196" s="2"/>
+      <c r="A196" s="11"/>
+      <c r="B196" s="15"/>
+      <c r="C196" s="11"/>
       <c r="D196" s="2"/>
       <c r="E196" s="2"/>
       <c r="F196" s="2"/>
       <c r="G196" s="2"/>
     </row>
     <row r="197" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A197" s="2"/>
-      <c r="B197" s="10"/>
-      <c r="C197" s="2"/>
+      <c r="A197" s="11"/>
+      <c r="B197" s="15"/>
+      <c r="C197" s="11"/>
       <c r="D197" s="2"/>
       <c r="E197" s="2"/>
       <c r="F197" s="2"/>
       <c r="G197" s="2"/>
     </row>
     <row r="198" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A198" s="2"/>
-      <c r="B198" s="10"/>
-      <c r="C198" s="2"/>
+      <c r="A198" s="11"/>
+      <c r="B198" s="15"/>
+      <c r="C198" s="11"/>
       <c r="D198" s="2"/>
       <c r="E198" s="2"/>
       <c r="F198" s="2"/>
       <c r="G198" s="2"/>
     </row>
     <row r="199" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A199" s="2"/>
-      <c r="B199" s="10"/>
-      <c r="C199" s="2"/>
+      <c r="A199" s="11"/>
+      <c r="B199" s="15"/>
+      <c r="C199" s="11"/>
       <c r="D199" s="2"/>
       <c r="E199" s="2"/>
       <c r="F199" s="2"/>
       <c r="G199" s="2"/>
     </row>
     <row r="200" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A200" s="2"/>
-      <c r="B200" s="10"/>
-      <c r="C200" s="2"/>
+      <c r="A200" s="11"/>
+      <c r="B200" s="15"/>
+      <c r="C200" s="11"/>
       <c r="D200" s="2"/>
       <c r="E200" s="2"/>
       <c r="F200" s="2"/>
       <c r="G200" s="2"/>
     </row>
     <row r="201" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A201" s="2"/>
-      <c r="B201" s="10"/>
-      <c r="C201" s="2"/>
+      <c r="A201" s="11"/>
+      <c r="B201" s="15"/>
+      <c r="C201" s="11"/>
       <c r="D201" s="2"/>
       <c r="E201" s="2"/>
       <c r="F201" s="2"/>
       <c r="G201" s="2"/>
     </row>
     <row r="202" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A202" s="2"/>
-      <c r="B202" s="10"/>
-      <c r="C202" s="2"/>
+      <c r="A202" s="11"/>
+      <c r="B202" s="15"/>
+      <c r="C202" s="11"/>
       <c r="D202" s="2"/>
       <c r="E202" s="2"/>
       <c r="F202" s="2"/>
       <c r="G202" s="2"/>
     </row>
     <row r="203" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A203" s="2"/>
-      <c r="B203" s="10"/>
-      <c r="C203" s="2"/>
+      <c r="A203" s="11"/>
+      <c r="B203" s="15"/>
+      <c r="C203" s="11"/>
       <c r="D203" s="2"/>
       <c r="E203" s="2"/>
       <c r="F203" s="2"/>
       <c r="G203" s="2"/>
     </row>
     <row r="204" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A204" s="2"/>
-      <c r="B204" s="10"/>
-      <c r="C204" s="2"/>
+      <c r="A204" s="11"/>
+      <c r="B204" s="15"/>
+      <c r="C204" s="11"/>
       <c r="D204" s="2"/>
       <c r="E204" s="2"/>
       <c r="F204" s="2"/>
       <c r="G204" s="2"/>
     </row>
     <row r="205" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A205" s="2"/>
-      <c r="B205" s="10"/>
-      <c r="C205" s="2"/>
+      <c r="A205" s="11"/>
+      <c r="B205" s="15"/>
+      <c r="C205" s="11"/>
       <c r="D205" s="2"/>
       <c r="E205" s="2"/>
       <c r="F205" s="2"/>
       <c r="G205" s="2"/>
     </row>
     <row r="206" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A206" s="2"/>
-      <c r="B206" s="10"/>
-      <c r="C206" s="2"/>
+      <c r="A206" s="11"/>
+      <c r="B206" s="15"/>
+      <c r="C206" s="11"/>
       <c r="D206" s="2"/>
       <c r="E206" s="2"/>
       <c r="F206" s="2"/>
       <c r="G206" s="2"/>
     </row>
     <row r="207" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A207" s="2"/>
-      <c r="B207" s="10"/>
-      <c r="C207" s="2"/>
+      <c r="A207" s="11"/>
+      <c r="B207" s="15"/>
+      <c r="C207" s="11"/>
       <c r="D207" s="2"/>
       <c r="E207" s="2"/>
       <c r="F207" s="2"/>
       <c r="G207" s="2"/>
     </row>
     <row r="208" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A208" s="2"/>
-      <c r="B208" s="10"/>
-      <c r="C208" s="2"/>
+      <c r="A208" s="11"/>
+      <c r="B208" s="15"/>
+      <c r="C208" s="11"/>
       <c r="D208" s="2"/>
       <c r="E208" s="2"/>
       <c r="F208" s="2"/>
       <c r="G208" s="2"/>
     </row>
     <row r="209" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A209" s="2"/>
-      <c r="B209" s="10"/>
-      <c r="C209" s="2"/>
+      <c r="A209" s="11"/>
+      <c r="B209" s="15"/>
+      <c r="C209" s="11"/>
       <c r="D209" s="2"/>
       <c r="E209" s="2"/>
       <c r="F209" s="2"/>
       <c r="G209" s="2"/>
     </row>
     <row r="210" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A210" s="2"/>
-      <c r="B210" s="10"/>
-      <c r="C210" s="2"/>
+      <c r="A210" s="11"/>
+      <c r="B210" s="15"/>
+      <c r="C210" s="11"/>
       <c r="D210" s="2"/>
       <c r="E210" s="2"/>
       <c r="F210" s="2"/>
       <c r="G210" s="2"/>
     </row>
     <row r="211" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A211" s="2"/>
-      <c r="B211" s="10"/>
-      <c r="C211" s="2"/>
+      <c r="A211" s="11"/>
+      <c r="B211" s="15"/>
+      <c r="C211" s="11"/>
       <c r="D211" s="2"/>
       <c r="E211" s="2"/>
       <c r="F211" s="2"/>
       <c r="G211" s="2"/>
     </row>
     <row r="212" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A212" s="2"/>
-      <c r="B212" s="10"/>
-      <c r="C212" s="2"/>
+      <c r="A212" s="11"/>
+      <c r="B212" s="15"/>
+      <c r="C212" s="11"/>
       <c r="D212" s="2"/>
       <c r="E212" s="2"/>
       <c r="F212" s="2"/>
       <c r="G212" s="2"/>
     </row>
     <row r="213" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A213" s="2"/>
-      <c r="B213" s="10"/>
-      <c r="C213" s="2"/>
+      <c r="A213" s="11"/>
+      <c r="B213" s="15"/>
+      <c r="C213" s="11"/>
       <c r="D213" s="2"/>
       <c r="E213" s="2"/>
       <c r="F213" s="2"/>
       <c r="G213" s="2"/>
     </row>
     <row r="214" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A214" s="2"/>
-      <c r="B214" s="10"/>
-      <c r="C214" s="2"/>
+      <c r="A214" s="11"/>
+      <c r="B214" s="15"/>
+      <c r="C214" s="11"/>
       <c r="D214" s="2"/>
       <c r="E214" s="2"/>
       <c r="F214" s="2"/>
       <c r="G214" s="2"/>
     </row>
     <row r="215" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A215" s="2"/>
-      <c r="B215" s="10"/>
-      <c r="C215" s="2"/>
+      <c r="A215" s="11"/>
+      <c r="B215" s="15"/>
+      <c r="C215" s="11"/>
       <c r="D215" s="2"/>
       <c r="E215" s="2"/>
       <c r="F215" s="2"/>
       <c r="G215" s="2"/>
     </row>
     <row r="216" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A216" s="2"/>
-      <c r="B216" s="10"/>
-      <c r="C216" s="2"/>
+      <c r="A216" s="11"/>
+      <c r="B216" s="15"/>
+      <c r="C216" s="11"/>
       <c r="D216" s="2"/>
       <c r="E216" s="2"/>
       <c r="F216" s="2"/>
       <c r="G216" s="2"/>
     </row>
     <row r="217" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A217" s="2"/>
-      <c r="B217" s="10"/>
-      <c r="C217" s="2"/>
+      <c r="A217" s="11"/>
+      <c r="B217" s="15"/>
+      <c r="C217" s="11"/>
       <c r="D217" s="2"/>
       <c r="E217" s="2"/>
       <c r="F217" s="2"/>
       <c r="G217" s="2"/>
     </row>
     <row r="218" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A218" s="2"/>
-      <c r="B218" s="10"/>
-      <c r="C218" s="2"/>
+      <c r="A218" s="11"/>
+      <c r="B218" s="15"/>
+      <c r="C218" s="11"/>
       <c r="D218" s="2"/>
       <c r="E218" s="2"/>
       <c r="F218" s="2"/>
       <c r="G218" s="2"/>
     </row>
     <row r="219" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A219" s="2"/>
-      <c r="B219" s="10"/>
-      <c r="C219" s="2"/>
+      <c r="A219" s="11"/>
+      <c r="B219" s="15"/>
+      <c r="C219" s="11"/>
       <c r="D219" s="2"/>
       <c r="E219" s="2"/>
       <c r="F219" s="2"/>
       <c r="G219" s="2"/>
     </row>
     <row r="220" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A220" s="2"/>
-      <c r="B220" s="10"/>
-      <c r="C220" s="2"/>
+      <c r="A220" s="11"/>
+      <c r="B220" s="15"/>
+      <c r="C220" s="11"/>
       <c r="D220" s="2"/>
       <c r="E220" s="2"/>
       <c r="F220" s="2"/>
       <c r="G220" s="2"/>
     </row>
     <row r="221" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A221" s="2"/>
-      <c r="B221" s="10"/>
-      <c r="C221" s="2"/>
+      <c r="A221" s="11"/>
+      <c r="B221" s="15"/>
+      <c r="C221" s="11"/>
       <c r="D221" s="2"/>
       <c r="E221" s="2"/>
       <c r="F221" s="2"/>
       <c r="G221" s="2"/>
     </row>
     <row r="222" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A222" s="2"/>
-      <c r="B222" s="10"/>
-      <c r="C222" s="2"/>
+      <c r="A222" s="11"/>
+      <c r="B222" s="15"/>
+      <c r="C222" s="11"/>
       <c r="D222" s="2"/>
       <c r="E222" s="2"/>
       <c r="F222" s="2"/>
       <c r="G222" s="2"/>
     </row>
     <row r="223" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A223" s="2"/>
-      <c r="B223" s="10"/>
-      <c r="C223" s="2"/>
+      <c r="A223" s="11"/>
+      <c r="B223" s="15"/>
+      <c r="C223" s="11"/>
       <c r="D223" s="2"/>
       <c r="E223" s="2"/>
       <c r="F223" s="2"/>
       <c r="G223" s="2"/>
     </row>
     <row r="224" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A224" s="2"/>
-      <c r="B224" s="10"/>
-      <c r="C224" s="2"/>
+      <c r="A224" s="11"/>
+      <c r="B224" s="15"/>
+      <c r="C224" s="11"/>
       <c r="D224" s="2"/>
       <c r="E224" s="2"/>
       <c r="F224" s="2"/>
       <c r="G224" s="2"/>
     </row>
     <row r="225" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A225" s="2"/>
-      <c r="B225" s="10"/>
-      <c r="C225" s="2"/>
+      <c r="A225" s="11"/>
+      <c r="B225" s="15"/>
+      <c r="C225" s="11"/>
       <c r="D225" s="2"/>
       <c r="E225" s="2"/>
       <c r="F225" s="2"/>
       <c r="G225" s="2"/>
     </row>
     <row r="226" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A226" s="2"/>
-      <c r="B226" s="10"/>
-      <c r="C226" s="2"/>
+      <c r="A226" s="11"/>
+      <c r="B226" s="15"/>
+      <c r="C226" s="11"/>
       <c r="D226" s="2"/>
       <c r="E226" s="2"/>
       <c r="F226" s="2"/>
       <c r="G226" s="2"/>
     </row>
     <row r="227" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A227" s="2"/>
-      <c r="B227" s="10"/>
-      <c r="C227" s="2"/>
+      <c r="A227" s="11"/>
+      <c r="B227" s="15"/>
+      <c r="C227" s="11"/>
       <c r="D227" s="2"/>
       <c r="E227" s="2"/>
       <c r="F227" s="2"/>
       <c r="G227" s="2"/>
     </row>
     <row r="228" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A228" s="2"/>
-      <c r="B228" s="10"/>
-      <c r="C228" s="2"/>
+      <c r="A228" s="11"/>
+      <c r="B228" s="15"/>
+      <c r="C228" s="11"/>
       <c r="D228" s="2"/>
       <c r="E228" s="2"/>
       <c r="F228" s="2"/>
       <c r="G228" s="2"/>
     </row>
     <row r="229" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A229" s="2"/>
-      <c r="B229" s="10"/>
-      <c r="C229" s="2"/>
+      <c r="A229" s="11"/>
+      <c r="B229" s="15"/>
+      <c r="C229" s="11"/>
       <c r="D229" s="2"/>
       <c r="E229" s="2"/>
       <c r="F229" s="2"/>
       <c r="G229" s="2"/>
     </row>
     <row r="230" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A230" s="2"/>
-      <c r="B230" s="10"/>
-      <c r="C230" s="2"/>
+      <c r="A230" s="11"/>
+      <c r="B230" s="15"/>
+      <c r="C230" s="11"/>
       <c r="D230" s="2"/>
       <c r="E230" s="2"/>
       <c r="F230" s="2"/>
       <c r="G230" s="2"/>
     </row>
     <row r="231" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A231" s="2"/>
-      <c r="B231" s="10"/>
-      <c r="C231" s="2"/>
+      <c r="A231" s="11"/>
+      <c r="B231" s="15"/>
+      <c r="C231" s="11"/>
       <c r="D231" s="2"/>
       <c r="E231" s="2"/>
       <c r="F231" s="2"/>
       <c r="G231" s="2"/>
     </row>
     <row r="232" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A232" s="2"/>
-      <c r="B232" s="10"/>
-      <c r="C232" s="2"/>
+      <c r="A232" s="11"/>
+      <c r="B232" s="15"/>
+      <c r="C232" s="11"/>
       <c r="D232" s="2"/>
       <c r="E232" s="2"/>
       <c r="F232" s="2"/>
       <c r="G232" s="2"/>
     </row>
     <row r="233" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A233" s="2"/>
-      <c r="B233" s="10"/>
-      <c r="C233" s="2"/>
+      <c r="A233" s="11"/>
+      <c r="B233" s="15"/>
+      <c r="C233" s="11"/>
       <c r="D233" s="2"/>
       <c r="E233" s="2"/>
       <c r="F233" s="2"/>
       <c r="G233" s="2"/>
     </row>
     <row r="234" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A234" s="2"/>
-      <c r="B234" s="10"/>
-      <c r="C234" s="2"/>
+      <c r="A234" s="11"/>
+      <c r="B234" s="15"/>
+      <c r="C234" s="11"/>
       <c r="D234" s="2"/>
       <c r="E234" s="2"/>
       <c r="F234" s="2"/>
       <c r="G234" s="2"/>
     </row>
     <row r="235" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A235" s="2"/>
-      <c r="B235" s="10"/>
-      <c r="C235" s="2"/>
+      <c r="A235" s="11"/>
+      <c r="B235" s="15"/>
+      <c r="C235" s="11"/>
       <c r="D235" s="2"/>
       <c r="E235" s="2"/>
       <c r="F235" s="2"/>
       <c r="G235" s="2"/>
     </row>
     <row r="236" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A236" s="2"/>
-      <c r="B236" s="10"/>
-      <c r="C236" s="2"/>
+      <c r="A236" s="11"/>
+      <c r="B236" s="15"/>
+      <c r="C236" s="11"/>
       <c r="D236" s="2"/>
       <c r="E236" s="2"/>
       <c r="F236" s="2"/>
       <c r="G236" s="2"/>
     </row>
     <row r="237" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A237" s="2"/>
-      <c r="B237" s="10"/>
-      <c r="C237" s="2"/>
+      <c r="A237" s="11"/>
+      <c r="B237" s="15"/>
+      <c r="C237" s="11"/>
       <c r="D237" s="2"/>
       <c r="E237" s="2"/>
       <c r="F237" s="2"/>
       <c r="G237" s="2"/>
     </row>
     <row r="238" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A238" s="2"/>
-      <c r="B238" s="10"/>
-      <c r="C238" s="2"/>
+      <c r="A238" s="11"/>
+      <c r="B238" s="15"/>
+      <c r="C238" s="11"/>
       <c r="D238" s="2"/>
       <c r="E238" s="2"/>
       <c r="F238" s="2"/>
       <c r="G238" s="2"/>
     </row>
     <row r="239" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A239" s="2"/>
-      <c r="B239" s="10"/>
-      <c r="C239" s="2"/>
+      <c r="A239" s="11"/>
+      <c r="B239" s="15"/>
+      <c r="C239" s="11"/>
       <c r="D239" s="2"/>
       <c r="E239" s="2"/>
       <c r="F239" s="2"/>
       <c r="G239" s="2"/>
     </row>
     <row r="240" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A240" s="2"/>
-      <c r="B240" s="10"/>
-      <c r="C240" s="2"/>
+      <c r="A240" s="11"/>
+      <c r="B240" s="15"/>
+      <c r="C240" s="11"/>
       <c r="D240" s="2"/>
       <c r="E240" s="2"/>
       <c r="F240" s="2"/>
       <c r="G240" s="2"/>
     </row>
     <row r="241" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A241" s="2"/>
-      <c r="B241" s="10"/>
-      <c r="C241" s="2"/>
+      <c r="A241" s="11"/>
+      <c r="B241" s="15"/>
+      <c r="C241" s="11"/>
       <c r="D241" s="2"/>
       <c r="E241" s="2"/>
       <c r="F241" s="2"/>
       <c r="G241" s="2"/>
     </row>
     <row r="242" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A242" s="2"/>
-      <c r="B242" s="10"/>
-      <c r="C242" s="2"/>
+      <c r="A242" s="11"/>
+      <c r="B242" s="15"/>
+      <c r="C242" s="11"/>
       <c r="D242" s="2"/>
       <c r="E242" s="2"/>
       <c r="F242" s="2"/>
       <c r="G242" s="2"/>
     </row>
     <row r="243" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A243" s="2"/>
-      <c r="B243" s="10"/>
-      <c r="C243" s="2"/>
+      <c r="A243" s="11"/>
+      <c r="B243" s="15"/>
+      <c r="C243" s="11"/>
       <c r="D243" s="2"/>
       <c r="E243" s="2"/>
       <c r="F243" s="2"/>
       <c r="G243" s="2"/>
     </row>
     <row r="244" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A244" s="2"/>
-      <c r="B244" s="10"/>
-      <c r="C244" s="2"/>
+      <c r="A244" s="11"/>
+      <c r="B244" s="15"/>
+      <c r="C244" s="11"/>
       <c r="D244" s="2"/>
       <c r="E244" s="2"/>
       <c r="F244" s="2"/>
       <c r="G244" s="2"/>
     </row>
     <row r="245" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A245" s="2"/>
-      <c r="B245" s="10"/>
-      <c r="C245" s="2"/>
+      <c r="A245" s="11"/>
+      <c r="B245" s="15"/>
+      <c r="C245" s="11"/>
       <c r="D245" s="2"/>
       <c r="E245" s="2"/>
       <c r="F245" s="2"/>
       <c r="G245" s="2"/>
     </row>
     <row r="246" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A246" s="2"/>
-      <c r="B246" s="10"/>
-      <c r="C246" s="2"/>
+      <c r="A246" s="11"/>
+      <c r="B246" s="15"/>
+      <c r="C246" s="11"/>
       <c r="D246" s="2"/>
       <c r="E246" s="2"/>
       <c r="F246" s="2"/>
       <c r="G246" s="2"/>
     </row>
     <row r="247" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A247" s="2"/>
-      <c r="B247" s="10"/>
-      <c r="C247" s="2"/>
+      <c r="A247" s="11"/>
+      <c r="B247" s="15"/>
+      <c r="C247" s="11"/>
       <c r="D247" s="2"/>
       <c r="E247" s="2"/>
       <c r="F247" s="2"/>
       <c r="G247" s="2"/>
     </row>
     <row r="248" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A248" s="2"/>
-      <c r="B248" s="10"/>
-      <c r="C248" s="2"/>
+      <c r="A248" s="11"/>
+      <c r="B248" s="15"/>
+      <c r="C248" s="11"/>
       <c r="D248" s="2"/>
       <c r="E248" s="2"/>
       <c r="F248" s="2"/>
       <c r="G248" s="2"/>
     </row>
     <row r="249" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A249" s="2"/>
-      <c r="B249" s="10"/>
-      <c r="C249" s="2"/>
+      <c r="A249" s="11"/>
+      <c r="B249" s="15"/>
+      <c r="C249" s="11"/>
       <c r="D249" s="2"/>
       <c r="E249" s="2"/>
       <c r="F249" s="2"/>
       <c r="G249" s="2"/>
     </row>
     <row r="250" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A250" s="2"/>
-      <c r="B250" s="10"/>
-      <c r="C250" s="2"/>
+      <c r="A250" s="11"/>
+      <c r="B250" s="15"/>
+      <c r="C250" s="11"/>
       <c r="D250" s="2"/>
       <c r="E250" s="2"/>
       <c r="F250" s="2"/>
       <c r="G250" s="2"/>
     </row>
     <row r="251" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A251" s="2"/>
-      <c r="B251" s="10"/>
-      <c r="C251" s="2"/>
+      <c r="A251" s="11"/>
+      <c r="B251" s="15"/>
+      <c r="C251" s="11"/>
       <c r="D251" s="2"/>
       <c r="E251" s="2"/>
       <c r="F251" s="2"/>
       <c r="G251" s="2"/>
     </row>
     <row r="252" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A252" s="2"/>
-      <c r="B252" s="10"/>
-      <c r="C252" s="2"/>
+      <c r="A252" s="11"/>
+      <c r="B252" s="15"/>
+      <c r="C252" s="11"/>
       <c r="D252" s="2"/>
       <c r="E252" s="2"/>
       <c r="F252" s="2"/>
       <c r="G252" s="2"/>
     </row>
     <row r="253" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A253" s="2"/>
-      <c r="B253" s="10"/>
-      <c r="C253" s="2"/>
+      <c r="A253" s="11"/>
+      <c r="B253" s="15"/>
+      <c r="C253" s="11"/>
       <c r="D253" s="2"/>
       <c r="E253" s="2"/>
       <c r="F253" s="2"/>
       <c r="G253" s="2"/>
     </row>
     <row r="254" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A254" s="2"/>
-      <c r="B254" s="10"/>
-      <c r="C254" s="2"/>
+      <c r="A254" s="11"/>
+      <c r="B254" s="15"/>
+      <c r="C254" s="11"/>
       <c r="D254" s="2"/>
       <c r="E254" s="2"/>
       <c r="F254" s="2"/>
       <c r="G254" s="2"/>
     </row>
     <row r="255" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A255" s="2"/>
-      <c r="B255" s="10"/>
-      <c r="C255" s="2"/>
+      <c r="A255" s="11"/>
+      <c r="B255" s="15"/>
+      <c r="C255" s="11"/>
       <c r="D255" s="2"/>
       <c r="E255" s="2"/>
       <c r="F255" s="2"/>
       <c r="G255" s="2"/>
     </row>
     <row r="256" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A256" s="2"/>
-      <c r="B256" s="10"/>
-      <c r="C256" s="2"/>
+      <c r="A256" s="11"/>
+      <c r="B256" s="15"/>
+      <c r="C256" s="11"/>
       <c r="D256" s="2"/>
       <c r="E256" s="2"/>
       <c r="F256" s="2"/>
       <c r="G256" s="2"/>
     </row>
     <row r="257" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A257" s="2"/>
-      <c r="B257" s="10"/>
-      <c r="C257" s="2"/>
+      <c r="A257" s="11"/>
+      <c r="B257" s="15"/>
+      <c r="C257" s="11"/>
       <c r="D257" s="2"/>
       <c r="E257" s="2"/>
       <c r="F257" s="2"/>
       <c r="G257" s="2"/>
     </row>
     <row r="258" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A258" s="2"/>
-      <c r="B258" s="10"/>
-      <c r="C258" s="2"/>
+      <c r="A258" s="11"/>
+      <c r="B258" s="15"/>
+      <c r="C258" s="11"/>
       <c r="D258" s="2"/>
       <c r="E258" s="2"/>
       <c r="F258" s="2"/>
       <c r="G258" s="2"/>
     </row>
     <row r="259" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A259" s="2"/>
-      <c r="B259" s="10"/>
-      <c r="C259" s="2"/>
+      <c r="A259" s="11"/>
+      <c r="B259" s="15"/>
+      <c r="C259" s="11"/>
       <c r="D259" s="2"/>
       <c r="E259" s="2"/>
       <c r="F259" s="2"/>
       <c r="G259" s="2"/>
     </row>
     <row r="260" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A260" s="2"/>
-      <c r="B260" s="10"/>
-      <c r="C260" s="2"/>
+      <c r="A260" s="11"/>
+      <c r="B260" s="15"/>
+      <c r="C260" s="11"/>
       <c r="D260" s="2"/>
       <c r="E260" s="2"/>
       <c r="F260" s="2"/>
       <c r="G260" s="2"/>
     </row>
     <row r="261" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A261" s="2"/>
-      <c r="B261" s="10"/>
-      <c r="C261" s="2"/>
+      <c r="A261" s="11"/>
+      <c r="B261" s="15"/>
+      <c r="C261" s="11"/>
       <c r="D261" s="2"/>
       <c r="E261" s="2"/>
       <c r="F261" s="2"/>
       <c r="G261" s="2"/>
     </row>
     <row r="262" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A262" s="2"/>
-      <c r="B262" s="10"/>
-      <c r="C262" s="2"/>
+      <c r="A262" s="11"/>
+      <c r="B262" s="15"/>
+      <c r="C262" s="11"/>
       <c r="D262" s="2"/>
       <c r="E262" s="2"/>
       <c r="F262" s="2"/>
       <c r="G262" s="2"/>
     </row>
     <row r="263" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A263" s="2"/>
-      <c r="B263" s="10"/>
-      <c r="C263" s="2"/>
+      <c r="A263" s="11"/>
+      <c r="B263" s="15"/>
+      <c r="C263" s="11"/>
       <c r="D263" s="2"/>
       <c r="E263" s="2"/>
       <c r="F263" s="2"/>
       <c r="G263" s="2"/>
     </row>
     <row r="264" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A264" s="2"/>
-      <c r="B264" s="10"/>
-      <c r="C264" s="2"/>
+      <c r="A264" s="11"/>
+      <c r="B264" s="15"/>
+      <c r="C264" s="11"/>
       <c r="D264" s="2"/>
       <c r="E264" s="2"/>
       <c r="F264" s="2"/>
       <c r="G264" s="2"/>
     </row>
     <row r="265" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A265" s="2"/>
-      <c r="B265" s="10"/>
-      <c r="C265" s="2"/>
+      <c r="A265" s="11"/>
+      <c r="B265" s="15"/>
+      <c r="C265" s="11"/>
       <c r="D265" s="2"/>
       <c r="E265" s="2"/>
       <c r="F265" s="2"/>
       <c r="G265" s="2"/>
     </row>
     <row r="266" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A266" s="2"/>
-      <c r="B266" s="10"/>
-      <c r="C266" s="2"/>
+      <c r="A266" s="11"/>
+      <c r="B266" s="15"/>
+      <c r="C266" s="11"/>
       <c r="D266" s="2"/>
       <c r="E266" s="2"/>
       <c r="F266" s="2"/>
       <c r="G266" s="2"/>
     </row>
     <row r="267" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A267" s="2"/>
-      <c r="B267" s="10"/>
-      <c r="C267" s="2"/>
+      <c r="A267" s="11"/>
+      <c r="B267" s="15"/>
+      <c r="C267" s="11"/>
       <c r="D267" s="2"/>
       <c r="E267" s="2"/>
       <c r="F267" s="2"/>
       <c r="G267" s="2"/>
     </row>
     <row r="268" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A268" s="2"/>
-      <c r="B268" s="10"/>
-      <c r="C268" s="2"/>
+      <c r="A268" s="11"/>
+      <c r="B268" s="15"/>
+      <c r="C268" s="11"/>
       <c r="D268" s="2"/>
       <c r="E268" s="2"/>
       <c r="F268" s="2"/>
       <c r="G268" s="2"/>
     </row>
     <row r="269" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A269" s="2"/>
-      <c r="B269" s="10"/>
-      <c r="C269" s="2"/>
+      <c r="A269" s="11"/>
+      <c r="B269" s="15"/>
+      <c r="C269" s="11"/>
       <c r="D269" s="2"/>
       <c r="E269" s="2"/>
       <c r="F269" s="2"/>
       <c r="G269" s="2"/>
     </row>
     <row r="270" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A270" s="2"/>
-      <c r="B270" s="10"/>
-      <c r="C270" s="2"/>
+      <c r="A270" s="11"/>
+      <c r="B270" s="15"/>
+      <c r="C270" s="11"/>
       <c r="D270" s="2"/>
       <c r="E270" s="2"/>
       <c r="F270" s="2"/>
       <c r="G270" s="2"/>
     </row>
     <row r="271" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A271" s="2"/>
-      <c r="B271" s="10"/>
-      <c r="C271" s="2"/>
+      <c r="A271" s="11"/>
+      <c r="B271" s="15"/>
+      <c r="C271" s="11"/>
       <c r="D271" s="2"/>
       <c r="E271" s="2"/>
       <c r="F271" s="2"/>
       <c r="G271" s="2"/>
     </row>
     <row r="272" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A272" s="2"/>
-      <c r="B272" s="10"/>
-      <c r="C272" s="2"/>
+      <c r="A272" s="11"/>
+      <c r="B272" s="15"/>
+      <c r="C272" s="11"/>
       <c r="D272" s="2"/>
       <c r="E272" s="2"/>
       <c r="F272" s="2"/>
       <c r="G272" s="2"/>
     </row>
     <row r="273" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A273" s="2"/>
-      <c r="B273" s="10"/>
-      <c r="C273" s="2"/>
+      <c r="A273" s="11"/>
+      <c r="B273" s="15"/>
+      <c r="C273" s="11"/>
       <c r="D273" s="2"/>
       <c r="E273" s="2"/>
       <c r="F273" s="2"/>
       <c r="G273" s="2"/>
     </row>
     <row r="274" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A274" s="2"/>
-      <c r="B274" s="10"/>
-      <c r="C274" s="2"/>
+      <c r="A274" s="11"/>
+      <c r="B274" s="15"/>
+      <c r="C274" s="11"/>
       <c r="D274" s="2"/>
       <c r="E274" s="2"/>
       <c r="F274" s="2"/>

</xml_diff>

<commit_message>
Update: Added Oprah, Coelho, etc
</commit_message>
<xml_diff>
--- a/All Other Data/s2cAllRawDataExcel.xlsx
+++ b/All Other Data/s2cAllRawDataExcel.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="112">
   <si>
     <t>Name</t>
   </si>
@@ -324,9 +324,6 @@
     <t>A Renaissance Polymath, Artist, Architect, Engineer, Inventor, Writer, Musician, Scientist. One of the greatest painters of all time. Credited with invention of helicopter, parachutes and tank. And of course drew The Last Supper and the Mona Lisa. His personality was considered to be "mysterious and remote".</t>
   </si>
   <si>
-    <t xml:space="preserve">Einstein’s parents wanted him to pursue a career in electrical engineering. Without a high school diploma, Einstein applied to the Polytechnic Institute at Zurich, Switzerland and failed the entrance examination although he got exceptional marks in the mathematics and physics sections. Einstein described himself as “a conscientious but unassuming young man who had acquired his meagre store of pertinent knowledge of the essentials through self study." Einstein basically taught himself math and physics through books and self-study and skipped lectures and stopped going to classes that didn't interest him. When he was working on the Theory of Relativity, he was working as an Assistant Examiner at a patent office. </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Suicidal Thoughts, Betrayal, Falsely Accused, Slandered, Persecuted, Early Death</t>
   </si>
   <si>
@@ -353,6 +350,69 @@
 I'll headlong leap from hell's high brink
        And wallow in its waves.'
 Lincoln, too, connected his mental well-being to divine forces. As a young man he saw how religion could ameliorate life's blows, even as he found the consolation of faith elusive. An infidel—a dissenter from orthodox Christianity—he resisted popular dogma. But many of history's greatest believers have also been its fiercest doubters. Lincoln charted his own theological course to a living vision of how frail, imperfect mortals could turn their suffering selves to the service of something greater and find solace—not in any personal satisfaction or glory but in dutiful mission.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Einstein was not able to speak until he was 4 years old and his teachers said "he would never amount to much". Einstein’s parents wanted him to pursue a career in electrical engineering. Without a high school diploma, Einstein applied to the Polytechnic Institute at Zurich, Switzerland and failed the entrance examination although he got exceptional marks in the mathematics and physics sections. Einstein described himself as “a conscientious but unassuming young man who had acquired his meagre store of pertinent knowledge of the essentials through self study." Einstein basically taught himself math and physics through books and self-study and skipped lectures and stopped going to classes that didn't interest him. When he was working on the Theory of Relativity, he was working as an Assistant Examiner at a patent office. And then of course, he became one of the greatest scientists of all time. </t>
+  </si>
+  <si>
+    <t>Steve Jobs</t>
+  </si>
+  <si>
+    <t>Depression, Mood Disorders, Lack of Formal Education</t>
+  </si>
+  <si>
+    <t>Steve Jobs was a famous college-dropout who was famous for his severe mood swings. At 30, he was left devastated and depressed after being fired from Apple, the very company he started. When Jobs looked back at this setback, he said this setback pushed him to "One of the most creative periods of his life" where he eventually founded Pixar and NextStep. His legacy is what allowed me to create this iOS app for you ;)</t>
+  </si>
+  <si>
+    <t>Walt Disney</t>
+  </si>
+  <si>
+    <t>Honda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disney was once fired from a newspaper company for "lacking imagination" and "having no original thoughts". 
+Goes to show that other people are a terrible judge of your internal potential ;) Probably because they don't know that 'what is essential is invisible to the eye' </t>
+  </si>
+  <si>
+    <t>Michael Jordan</t>
+  </si>
+  <si>
+    <t>He was cut from his HS basketball team and apparently went home, locked himself in his room and cried. 
+And those tears then propelled him into becoming the greatest basketball player of all-time.</t>
+  </si>
+  <si>
+    <t>Paulo Coelho</t>
+  </si>
+  <si>
+    <t>Rejection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"The Alchemist" was rejected over 200 times before it went on to sell 75 Million cpies. </t>
+  </si>
+  <si>
+    <t>Oprah Winfrey</t>
+  </si>
+  <si>
+    <t>Richard Pryor</t>
+  </si>
+  <si>
+    <t>Rodney Dangerfield</t>
+  </si>
+  <si>
+    <t>Jim Carrey</t>
+  </si>
+  <si>
+    <t>Poverty, Depression</t>
+  </si>
+  <si>
+    <t>Childhood abuse, Stage Fright</t>
+  </si>
+  <si>
+    <t>Childhood abuse</t>
+  </si>
+  <si>
+    <t>Oprah was sexualy abused by male relatives of her family during adolescence. 
+Today, she is one of the most beloved TV show talk hosts, actress, publisher, producer and philanthropist.</t>
   </si>
 </sst>
 </file>
@@ -793,10 +853,10 @@
   <dimension ref="A1:G274"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -841,17 +901,17 @@
         <v>51</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>52</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="409" x14ac:dyDescent="0.35">
@@ -868,7 +928,7 @@
         <v>30</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="F3" s="16" t="s">
         <v>33</v>
@@ -940,13 +1000,13 @@
         <v>50</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>55</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -1175,7 +1235,7 @@
     </row>
     <row r="20" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B20" s="12"/>
       <c r="C20" s="9"/>
@@ -1186,7 +1246,7 @@
     </row>
     <row r="21" spans="1:7" ht="31" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B21" s="12"/>
       <c r="C21" s="9"/>
@@ -1195,26 +1255,38 @@
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A22" s="9"/>
+    <row r="22" spans="1:7" ht="248" x14ac:dyDescent="0.35">
+      <c r="A22" s="9" t="s">
+        <v>93</v>
+      </c>
       <c r="B22" s="12"/>
-      <c r="C22" s="9"/>
+      <c r="C22" s="9" t="s">
+        <v>94</v>
+      </c>
       <c r="D22" s="9"/>
-      <c r="E22" s="2"/>
+      <c r="E22" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A23" s="9"/>
+    <row r="23" spans="1:7" ht="155" x14ac:dyDescent="0.35">
+      <c r="A23" s="9" t="s">
+        <v>96</v>
+      </c>
       <c r="B23" s="12"/>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
-      <c r="E23" s="2"/>
+      <c r="E23" s="2" t="s">
+        <v>98</v>
+      </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
     <row r="24" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A24" s="9"/>
+      <c r="A24" s="9" t="s">
+        <v>97</v>
+      </c>
       <c r="B24" s="12"/>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
@@ -1222,55 +1294,85 @@
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A25" s="9"/>
+    <row r="25" spans="1:7" ht="124" x14ac:dyDescent="0.35">
+      <c r="A25" s="9" t="s">
+        <v>99</v>
+      </c>
       <c r="B25" s="12"/>
-      <c r="C25" s="9"/>
+      <c r="C25" s="9" t="s">
+        <v>70</v>
+      </c>
       <c r="D25" s="9"/>
-      <c r="E25" s="2"/>
+      <c r="E25" s="2" t="s">
+        <v>100</v>
+      </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A26" s="9"/>
+    <row r="26" spans="1:7" ht="62" x14ac:dyDescent="0.35">
+      <c r="A26" s="9" t="s">
+        <v>101</v>
+      </c>
       <c r="B26" s="12"/>
-      <c r="C26" s="9"/>
+      <c r="C26" s="9" t="s">
+        <v>102</v>
+      </c>
       <c r="D26" s="9"/>
-      <c r="E26" s="2"/>
+      <c r="E26" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A27" s="9"/>
+    <row r="27" spans="1:7" ht="124" x14ac:dyDescent="0.35">
+      <c r="A27" s="9" t="s">
+        <v>104</v>
+      </c>
       <c r="B27" s="12"/>
-      <c r="C27" s="9"/>
+      <c r="C27" s="9" t="s">
+        <v>110</v>
+      </c>
       <c r="D27" s="9"/>
-      <c r="E27" s="2"/>
+      <c r="E27" s="2" t="s">
+        <v>111</v>
+      </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A28" s="9"/>
+    <row r="28" spans="1:7" ht="62" x14ac:dyDescent="0.35">
+      <c r="A28" s="9" t="s">
+        <v>105</v>
+      </c>
       <c r="B28" s="12"/>
-      <c r="C28" s="9"/>
+      <c r="C28" s="9" t="s">
+        <v>109</v>
+      </c>
       <c r="D28" s="9"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A29" s="9"/>
+      <c r="A29" s="9" t="s">
+        <v>106</v>
+      </c>
       <c r="B29" s="12"/>
-      <c r="C29" s="9"/>
+      <c r="C29" s="9" t="s">
+        <v>70</v>
+      </c>
       <c r="D29" s="9"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
     </row>
     <row r="30" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A30" s="9"/>
+      <c r="A30" s="9" t="s">
+        <v>107</v>
+      </c>
       <c r="B30" s="12"/>
-      <c r="C30" s="9"/>
+      <c r="C30" s="9" t="s">
+        <v>108</v>
+      </c>
       <c r="D30" s="9"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>

</xml_diff>